<commit_message>
leftovers from first deploy
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAjoku\Documents\GitHub\GCGRrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E3C22-7C31-4B16-89A9-C3D44656DE4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB6FC4-943B-4204-BCEC-6A5B0EACC62C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="7020" xr2:uid="{2E80CA58-8610-40E9-A54D-09997D7EA2F4}"/>
   </bookViews>
@@ -8151,6 +8151,22 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
@@ -8159,14 +8175,6 @@
       <alignment horizontal="left" vertical="top" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -8188,14 +8196,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -20551,7 +20551,7 @@
       </c>
       <c r="D11" s="12">
         <f ca="1">NOW()</f>
-        <v>43325.678335185185</v>
+        <v>43325.689186226853</v>
       </c>
       <c r="E11" s="315"/>
       <c r="F11" s="313"/>
@@ -21047,7 +21047,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43325.678335185185</v>
+        <v>43325.689186226853</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>
@@ -34491,10 +34491,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -34575,11 +34575,11 @@
       <c r="AM1" s="321"/>
     </row>
     <row r="2" spans="1:43" s="311" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="688" t="str">
+      <c r="B2" s="692" t="str">
         <f>IF(Settings!D4&lt;&gt;0,Settings!D4,"")</f>
         <v/>
       </c>
-      <c r="C2" s="688"/>
+      <c r="C2" s="692"/>
       <c r="D2" s="324"/>
       <c r="G2" s="325"/>
       <c r="AB2" s="326"/>
@@ -34591,15 +34591,15 @@
       <c r="AQ2" s="321"/>
     </row>
     <row r="3" spans="1:43" s="311" customFormat="1" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="689" t="str">
+      <c r="B3" s="693" t="str">
         <f>IF(Settings!D5&lt;&gt;0,Settings!D5,"")</f>
         <v/>
       </c>
-      <c r="C3" s="689"/>
+      <c r="C3" s="693"/>
       <c r="D3" s="327"/>
       <c r="E3" s="328">
         <f ca="1">Settings!\date</f>
-        <v>43325.678335185185</v>
+        <v>43325.689186226853</v>
       </c>
       <c r="Q3" s="326"/>
       <c r="AD3" s="326"/>
@@ -34826,18 +34826,18 @@
       <c r="B11" s="351"/>
       <c r="C11" s="352"/>
       <c r="D11" s="352"/>
-      <c r="E11" s="692" t="s">
+      <c r="E11" s="694" t="s">
         <v>245</v>
       </c>
       <c r="F11" s="352"/>
-      <c r="G11" s="692" t="s">
+      <c r="G11" s="694" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="352"/>
-      <c r="I11" s="692" t="s">
+      <c r="I11" s="694" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="692" t="s">
+      <c r="J11" s="694" t="s">
         <v>246</v>
       </c>
       <c r="K11" s="353"/>
@@ -34849,40 +34849,40 @@
       </c>
       <c r="O11" s="359"/>
       <c r="P11" s="360"/>
-      <c r="Q11" s="694" t="s">
+      <c r="Q11" s="696" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="698" t="s">
+      <c r="R11" s="690" t="s">
         <v>368</v>
       </c>
-      <c r="S11" s="696" t="s">
+      <c r="S11" s="698" t="s">
         <v>369</v>
       </c>
-      <c r="T11" s="690" t="s">
+      <c r="T11" s="688" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="690" t="s">
+      <c r="U11" s="688" t="s">
         <v>234</v>
       </c>
-      <c r="V11" s="690" t="s">
+      <c r="V11" s="688" t="s">
         <v>235</v>
       </c>
-      <c r="W11" s="690" t="s">
+      <c r="W11" s="688" t="s">
         <v>239</v>
       </c>
-      <c r="X11" s="690" t="s">
+      <c r="X11" s="688" t="s">
         <v>237</v>
       </c>
-      <c r="Y11" s="690" t="s">
+      <c r="Y11" s="688" t="s">
         <v>238</v>
       </c>
-      <c r="Z11" s="690" t="s">
+      <c r="Z11" s="688" t="s">
         <v>241</v>
       </c>
-      <c r="AA11" s="690" t="s">
+      <c r="AA11" s="688" t="s">
         <v>240</v>
       </c>
-      <c r="AB11" s="690" t="s">
+      <c r="AB11" s="688" t="s">
         <v>236</v>
       </c>
       <c r="AC11" s="361"/>
@@ -34906,14 +34906,14 @@
       <c r="D12" s="365" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="693"/>
+      <c r="E12" s="695"/>
       <c r="F12" s="365"/>
-      <c r="G12" s="693"/>
+      <c r="G12" s="695"/>
       <c r="H12" s="365" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="693"/>
-      <c r="J12" s="693"/>
+      <c r="I12" s="695"/>
+      <c r="J12" s="695"/>
       <c r="K12" s="366" t="s">
         <v>232</v>
       </c>
@@ -34928,18 +34928,18 @@
       <c r="P12" s="373" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="695"/>
-      <c r="R12" s="699"/>
-      <c r="S12" s="697"/>
-      <c r="T12" s="691"/>
-      <c r="U12" s="691"/>
-      <c r="V12" s="691"/>
-      <c r="W12" s="691"/>
-      <c r="X12" s="691"/>
-      <c r="Y12" s="691"/>
-      <c r="Z12" s="691"/>
-      <c r="AA12" s="691"/>
-      <c r="AB12" s="691"/>
+      <c r="Q12" s="697"/>
+      <c r="R12" s="691"/>
+      <c r="S12" s="699"/>
+      <c r="T12" s="689"/>
+      <c r="U12" s="689"/>
+      <c r="V12" s="689"/>
+      <c r="W12" s="689"/>
+      <c r="X12" s="689"/>
+      <c r="Y12" s="689"/>
+      <c r="Z12" s="689"/>
+      <c r="AA12" s="689"/>
+      <c r="AB12" s="689"/>
       <c r="AC12" s="374"/>
       <c r="AD12" s="375" t="s">
         <v>2</v>
@@ -37461,13 +37461,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="18">
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="W11:W12"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="U11:U12"/>
@@ -37479,6 +37472,13 @@
     <mergeCell ref="Q11:Q12"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="S11:S12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="W11:W12"/>
   </mergeCells>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="11" priority="4">
@@ -54436,7 +54436,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43325.678335185185</v>
+        <v>43325.689186226853</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>

</xml_diff>

<commit_message>
Revert "leftovers from first deploy"
This reverts commit a18123c5b8f66a786cf2997e1ccc8ee5e10d4d42.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAjoku\Documents\GitHub\GCGRrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB6FC4-943B-4204-BCEC-6A5B0EACC62C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1E3C22-7C31-4B16-89A9-C3D44656DE4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="7020" xr2:uid="{2E80CA58-8610-40E9-A54D-09997D7EA2F4}"/>
   </bookViews>
@@ -8151,6 +8151,14 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="2"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -8159,43 +8167,35 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="2"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -20551,7 +20551,7 @@
       </c>
       <c r="D11" s="12">
         <f ca="1">NOW()</f>
-        <v>43325.689186226853</v>
+        <v>43325.678335185185</v>
       </c>
       <c r="E11" s="315"/>
       <c r="F11" s="313"/>
@@ -21047,7 +21047,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43325.689186226853</v>
+        <v>43325.678335185185</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>
@@ -34491,10 +34491,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -34575,11 +34575,11 @@
       <c r="AM1" s="321"/>
     </row>
     <row r="2" spans="1:43" s="311" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="692" t="str">
+      <c r="B2" s="688" t="str">
         <f>IF(Settings!D4&lt;&gt;0,Settings!D4,"")</f>
         <v/>
       </c>
-      <c r="C2" s="692"/>
+      <c r="C2" s="688"/>
       <c r="D2" s="324"/>
       <c r="G2" s="325"/>
       <c r="AB2" s="326"/>
@@ -34591,15 +34591,15 @@
       <c r="AQ2" s="321"/>
     </row>
     <row r="3" spans="1:43" s="311" customFormat="1" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="693" t="str">
+      <c r="B3" s="689" t="str">
         <f>IF(Settings!D5&lt;&gt;0,Settings!D5,"")</f>
         <v/>
       </c>
-      <c r="C3" s="693"/>
+      <c r="C3" s="689"/>
       <c r="D3" s="327"/>
       <c r="E3" s="328">
         <f ca="1">Settings!\date</f>
-        <v>43325.689186226853</v>
+        <v>43325.678335185185</v>
       </c>
       <c r="Q3" s="326"/>
       <c r="AD3" s="326"/>
@@ -34826,18 +34826,18 @@
       <c r="B11" s="351"/>
       <c r="C11" s="352"/>
       <c r="D11" s="352"/>
-      <c r="E11" s="694" t="s">
+      <c r="E11" s="692" t="s">
         <v>245</v>
       </c>
       <c r="F11" s="352"/>
-      <c r="G11" s="694" t="s">
+      <c r="G11" s="692" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="352"/>
-      <c r="I11" s="694" t="s">
+      <c r="I11" s="692" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="694" t="s">
+      <c r="J11" s="692" t="s">
         <v>246</v>
       </c>
       <c r="K11" s="353"/>
@@ -34849,40 +34849,40 @@
       </c>
       <c r="O11" s="359"/>
       <c r="P11" s="360"/>
-      <c r="Q11" s="696" t="s">
+      <c r="Q11" s="694" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="690" t="s">
+      <c r="R11" s="698" t="s">
         <v>368</v>
       </c>
-      <c r="S11" s="698" t="s">
+      <c r="S11" s="696" t="s">
         <v>369</v>
       </c>
-      <c r="T11" s="688" t="s">
+      <c r="T11" s="690" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="688" t="s">
+      <c r="U11" s="690" t="s">
         <v>234</v>
       </c>
-      <c r="V11" s="688" t="s">
+      <c r="V11" s="690" t="s">
         <v>235</v>
       </c>
-      <c r="W11" s="688" t="s">
+      <c r="W11" s="690" t="s">
         <v>239</v>
       </c>
-      <c r="X11" s="688" t="s">
+      <c r="X11" s="690" t="s">
         <v>237</v>
       </c>
-      <c r="Y11" s="688" t="s">
+      <c r="Y11" s="690" t="s">
         <v>238</v>
       </c>
-      <c r="Z11" s="688" t="s">
+      <c r="Z11" s="690" t="s">
         <v>241</v>
       </c>
-      <c r="AA11" s="688" t="s">
+      <c r="AA11" s="690" t="s">
         <v>240</v>
       </c>
-      <c r="AB11" s="688" t="s">
+      <c r="AB11" s="690" t="s">
         <v>236</v>
       </c>
       <c r="AC11" s="361"/>
@@ -34906,14 +34906,14 @@
       <c r="D12" s="365" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="695"/>
+      <c r="E12" s="693"/>
       <c r="F12" s="365"/>
-      <c r="G12" s="695"/>
+      <c r="G12" s="693"/>
       <c r="H12" s="365" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="695"/>
-      <c r="J12" s="695"/>
+      <c r="I12" s="693"/>
+      <c r="J12" s="693"/>
       <c r="K12" s="366" t="s">
         <v>232</v>
       </c>
@@ -34928,18 +34928,18 @@
       <c r="P12" s="373" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="697"/>
-      <c r="R12" s="691"/>
-      <c r="S12" s="699"/>
-      <c r="T12" s="689"/>
-      <c r="U12" s="689"/>
-      <c r="V12" s="689"/>
-      <c r="W12" s="689"/>
-      <c r="X12" s="689"/>
-      <c r="Y12" s="689"/>
-      <c r="Z12" s="689"/>
-      <c r="AA12" s="689"/>
-      <c r="AB12" s="689"/>
+      <c r="Q12" s="695"/>
+      <c r="R12" s="699"/>
+      <c r="S12" s="697"/>
+      <c r="T12" s="691"/>
+      <c r="U12" s="691"/>
+      <c r="V12" s="691"/>
+      <c r="W12" s="691"/>
+      <c r="X12" s="691"/>
+      <c r="Y12" s="691"/>
+      <c r="Z12" s="691"/>
+      <c r="AA12" s="691"/>
+      <c r="AB12" s="691"/>
       <c r="AC12" s="374"/>
       <c r="AD12" s="375" t="s">
         <v>2</v>
@@ -37461,6 +37461,13 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="18">
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="W11:W12"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="U11:U12"/>
@@ -37472,13 +37479,6 @@
     <mergeCell ref="Q11:Q12"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="S11:S12"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="W11:W12"/>
   </mergeCells>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="11" priority="4">
@@ -54436,7 +54436,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43325.689186226853</v>
+        <v>43325.678335185185</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>

</xml_diff>

<commit_message>
added updated template bc I couldn't execute pull request from develop
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAjoku\Documents\GitHub\GCGRrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D062238-2D6D-42BA-BC54-BC5A1F0ABA83}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA0BB24-6BCE-4CFC-BAC2-C6EED18B3AD1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="7020" xr2:uid="{2E80CA58-8610-40E9-A54D-09997D7EA2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="3" r:id="rId1"/>
     <sheet name="meta" sheetId="36" state="veryHidden" r:id="rId2"/>
-    <sheet name="Staff Detail" sheetId="1" r:id="rId3"/>
+    <sheet name="Staff Detail" sheetId="1" state="hidden" r:id="rId3"/>
     <sheet name="Labor Gantt" sheetId="30" state="hidden" r:id="rId4"/>
     <sheet name="Non-Staff Labor" sheetId="34" state="hidden" r:id="rId5"/>
     <sheet name="Rate Tables" sheetId="35" state="hidden" r:id="rId6"/>
@@ -6089,7 +6089,7 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="710">
+  <cellXfs count="709">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -8127,10 +8127,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="77" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -8225,12 +8228,6 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -20362,8 +20359,8 @@
       <c r="C4" s="314" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="685"/>
-      <c r="E4" s="686"/>
+      <c r="D4" s="686"/>
+      <c r="E4" s="687"/>
       <c r="F4" s="315"/>
       <c r="G4" s="314" t="s">
         <v>207</v>
@@ -20390,8 +20387,8 @@
       <c r="C5" s="314" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="685"/>
-      <c r="E5" s="686"/>
+      <c r="D5" s="686"/>
+      <c r="E5" s="687"/>
       <c r="F5" s="315"/>
       <c r="G5" s="314" t="s">
         <v>208</v>
@@ -20418,10 +20415,10 @@
       <c r="C6" s="314" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="685" t="s">
+      <c r="D6" s="686" t="s">
         <v>274</v>
       </c>
-      <c r="E6" s="686"/>
+      <c r="E6" s="687"/>
       <c r="F6" s="315"/>
       <c r="G6" s="314" t="s">
         <v>9</v>
@@ -20431,7 +20428,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I6" s="315"/>
-      <c r="J6" s="687" t="s">
+      <c r="J6" s="688" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="514" t="e">
@@ -20454,10 +20451,10 @@
       <c r="C7" s="314" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="683" t="s">
+      <c r="D7" s="684" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="684"/>
+      <c r="E7" s="685"/>
       <c r="F7" s="315"/>
       <c r="G7" s="315"/>
       <c r="H7" s="515" t="e">
@@ -20465,7 +20462,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="687"/>
+      <c r="J7" s="688"/>
       <c r="K7" s="515" t="e">
         <f ca="1">IF(cDateDiff("WW",\cstart,\cend)&gt;0,cDateDiff("WW",\cstart,\cend),0)</f>
         <v>#NAME?</v>
@@ -20557,7 +20554,7 @@
       </c>
       <c r="D11" s="12">
         <f ca="1">NOW()</f>
-        <v>43326.474299305555</v>
+        <v>43327.344405324075</v>
       </c>
       <c r="E11" s="315"/>
       <c r="F11" s="313"/>
@@ -20675,10 +20672,10 @@
       <c r="C16" s="314" t="s">
         <v>227</v>
       </c>
-      <c r="D16" s="685" t="s">
+      <c r="D16" s="686" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="686"/>
+      <c r="E16" s="687"/>
       <c r="F16" s="315"/>
       <c r="G16" s="314" t="s">
         <v>226</v>
@@ -21053,7 +21050,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43326.474299305555</v>
+        <v>43327.344405324075</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>
@@ -34482,12 +34479,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1A4F89-FC04-4A38-97E9-6714BC2884DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F093129-0C35-4C29-B2A0-FFC991FE5B09}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34497,7 +34494,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -34518,7 +34515,7 @@
     <sheetView showZeros="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="12" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:C2"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -34581,11 +34578,11 @@
       <c r="AM1" s="321"/>
     </row>
     <row r="2" spans="1:43" s="311" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="688" t="str">
+      <c r="B2" s="689" t="str">
         <f>IF(Settings!D4&lt;&gt;0,Settings!D4,"")</f>
         <v/>
       </c>
-      <c r="C2" s="688"/>
+      <c r="C2" s="689"/>
       <c r="D2" s="324"/>
       <c r="G2" s="325"/>
       <c r="AB2" s="326"/>
@@ -34597,15 +34594,15 @@
       <c r="AQ2" s="321"/>
     </row>
     <row r="3" spans="1:43" s="311" customFormat="1" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="689" t="str">
+      <c r="B3" s="690" t="str">
         <f>IF(Settings!D5&lt;&gt;0,Settings!D5,"")</f>
         <v/>
       </c>
-      <c r="C3" s="689"/>
+      <c r="C3" s="690"/>
       <c r="D3" s="327"/>
       <c r="E3" s="328">
         <f ca="1">Settings!\date</f>
-        <v>43326.474299305555</v>
+        <v>43327.344405324075</v>
       </c>
       <c r="Q3" s="326"/>
       <c r="AD3" s="326"/>
@@ -34832,18 +34829,18 @@
       <c r="B11" s="351"/>
       <c r="C11" s="352"/>
       <c r="D11" s="352"/>
-      <c r="E11" s="692" t="s">
+      <c r="E11" s="693" t="s">
         <v>245</v>
       </c>
       <c r="F11" s="352"/>
-      <c r="G11" s="692" t="s">
+      <c r="G11" s="693" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="352"/>
-      <c r="I11" s="692" t="s">
+      <c r="I11" s="693" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="692" t="s">
+      <c r="J11" s="693" t="s">
         <v>246</v>
       </c>
       <c r="K11" s="353"/>
@@ -34855,40 +34852,40 @@
       </c>
       <c r="O11" s="359"/>
       <c r="P11" s="360"/>
-      <c r="Q11" s="694" t="s">
+      <c r="Q11" s="695" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="698" t="s">
+      <c r="R11" s="699" t="s">
         <v>368</v>
       </c>
-      <c r="S11" s="696" t="s">
+      <c r="S11" s="697" t="s">
         <v>369</v>
       </c>
-      <c r="T11" s="690" t="s">
+      <c r="T11" s="691" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="690" t="s">
+      <c r="U11" s="691" t="s">
         <v>234</v>
       </c>
-      <c r="V11" s="690" t="s">
+      <c r="V11" s="691" t="s">
         <v>235</v>
       </c>
-      <c r="W11" s="690" t="s">
+      <c r="W11" s="691" t="s">
         <v>239</v>
       </c>
-      <c r="X11" s="690" t="s">
+      <c r="X11" s="691" t="s">
         <v>237</v>
       </c>
-      <c r="Y11" s="690" t="s">
+      <c r="Y11" s="691" t="s">
         <v>238</v>
       </c>
-      <c r="Z11" s="690" t="s">
+      <c r="Z11" s="691" t="s">
         <v>241</v>
       </c>
-      <c r="AA11" s="690" t="s">
+      <c r="AA11" s="691" t="s">
         <v>240</v>
       </c>
-      <c r="AB11" s="690" t="s">
+      <c r="AB11" s="691" t="s">
         <v>236</v>
       </c>
       <c r="AC11" s="361"/>
@@ -34912,14 +34909,14 @@
       <c r="D12" s="365" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="693"/>
+      <c r="E12" s="694"/>
       <c r="F12" s="365"/>
-      <c r="G12" s="693"/>
+      <c r="G12" s="694"/>
       <c r="H12" s="365" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="693"/>
-      <c r="J12" s="693"/>
+      <c r="I12" s="694"/>
+      <c r="J12" s="694"/>
       <c r="K12" s="366" t="s">
         <v>232</v>
       </c>
@@ -34934,18 +34931,18 @@
       <c r="P12" s="373" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="695"/>
-      <c r="R12" s="699"/>
-      <c r="S12" s="697"/>
-      <c r="T12" s="691"/>
-      <c r="U12" s="691"/>
-      <c r="V12" s="691"/>
-      <c r="W12" s="691"/>
-      <c r="X12" s="691"/>
-      <c r="Y12" s="691"/>
-      <c r="Z12" s="691"/>
-      <c r="AA12" s="691"/>
-      <c r="AB12" s="691"/>
+      <c r="Q12" s="696"/>
+      <c r="R12" s="700"/>
+      <c r="S12" s="698"/>
+      <c r="T12" s="692"/>
+      <c r="U12" s="692"/>
+      <c r="V12" s="692"/>
+      <c r="W12" s="692"/>
+      <c r="X12" s="692"/>
+      <c r="Y12" s="692"/>
+      <c r="Z12" s="692"/>
+      <c r="AA12" s="692"/>
+      <c r="AB12" s="692"/>
       <c r="AC12" s="374"/>
       <c r="AD12" s="375" t="s">
         <v>2</v>
@@ -37538,22 +37535,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="I1" s="700"/>
-      <c r="J1" s="700"/>
-      <c r="K1" s="700"/>
-      <c r="L1" s="700"/>
-      <c r="M1" s="700"/>
-      <c r="N1" s="700"/>
-      <c r="O1" s="700"/>
-      <c r="P1" s="700"/>
-      <c r="Q1" s="700"/>
-      <c r="R1" s="700"/>
-      <c r="S1" s="700"/>
-      <c r="T1" s="700"/>
-      <c r="U1" s="700"/>
-      <c r="V1" s="700"/>
-      <c r="W1" s="700"/>
-      <c r="X1" s="700"/>
+      <c r="I1" s="701"/>
+      <c r="J1" s="701"/>
+      <c r="K1" s="701"/>
+      <c r="L1" s="701"/>
+      <c r="M1" s="701"/>
+      <c r="N1" s="701"/>
+      <c r="O1" s="701"/>
+      <c r="P1" s="701"/>
+      <c r="Q1" s="701"/>
+      <c r="R1" s="701"/>
+      <c r="S1" s="701"/>
+      <c r="T1" s="701"/>
+      <c r="U1" s="701"/>
+      <c r="V1" s="701"/>
+      <c r="W1" s="701"/>
+      <c r="X1" s="701"/>
       <c r="Y1" s="608"/>
       <c r="Z1" s="608"/>
       <c r="AA1" s="608"/>
@@ -38054,7 +38051,7 @@
       <c r="CL8" s="634"/>
       <c r="CM8" s="634"/>
       <c r="CN8" s="634"/>
-      <c r="CO8" s="634"/>
+      <c r="CO8" s="639"/>
       <c r="CP8" s="623"/>
       <c r="CR8" s="634"/>
     </row>
@@ -38277,7 +38274,7 @@
       </c>
       <c r="G11" s="651"/>
       <c r="H11" s="652"/>
-      <c r="I11" s="708"/>
+      <c r="I11" s="682"/>
       <c r="J11" s="607"/>
       <c r="K11" s="607"/>
       <c r="L11" s="607"/>
@@ -38361,9 +38358,9 @@
       <c r="CL11" s="607"/>
       <c r="CM11" s="607"/>
       <c r="CN11" s="607"/>
-      <c r="CO11" s="709"/>
+      <c r="CO11" s="683"/>
       <c r="CP11" s="623"/>
-      <c r="CR11" s="681"/>
+      <c r="CR11" s="607"/>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="B12" s="606"/>
@@ -39385,13 +39382,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="U1" s="701"/>
-      <c r="V1" s="701"/>
-      <c r="W1" s="701"/>
-      <c r="AJ1" s="701"/>
-      <c r="AK1" s="701"/>
-      <c r="AL1" s="701"/>
-      <c r="AM1" s="701"/>
+      <c r="U1" s="702"/>
+      <c r="V1" s="702"/>
+      <c r="W1" s="702"/>
+      <c r="AJ1" s="702"/>
+      <c r="AK1" s="702"/>
+      <c r="AL1" s="702"/>
+      <c r="AM1" s="702"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="H6" s="672"/>
@@ -39405,43 +39402,43 @@
       <c r="C11" s="57"/>
       <c r="D11" s="264"/>
       <c r="E11" s="265"/>
-      <c r="F11" s="702" t="s">
+      <c r="F11" s="703" t="s">
         <v>1009</v>
       </c>
-      <c r="G11" s="702"/>
-      <c r="H11" s="702"/>
-      <c r="I11" s="703" t="s">
+      <c r="G11" s="703"/>
+      <c r="H11" s="703"/>
+      <c r="I11" s="704" t="s">
         <v>470</v>
       </c>
-      <c r="J11" s="703"/>
-      <c r="K11" s="703"/>
-      <c r="L11" s="703" t="s">
+      <c r="J11" s="704"/>
+      <c r="K11" s="704"/>
+      <c r="L11" s="704" t="s">
         <v>364</v>
       </c>
-      <c r="M11" s="703"/>
-      <c r="N11" s="703"/>
-      <c r="O11" s="703" t="s">
+      <c r="M11" s="704"/>
+      <c r="N11" s="704"/>
+      <c r="O11" s="704" t="s">
         <v>1010</v>
       </c>
-      <c r="P11" s="703"/>
-      <c r="Q11" s="703"/>
-      <c r="R11" s="703" t="s">
+      <c r="P11" s="704"/>
+      <c r="Q11" s="704"/>
+      <c r="R11" s="704" t="s">
         <v>1011</v>
       </c>
-      <c r="S11" s="703"/>
-      <c r="T11" s="703"/>
-      <c r="U11" s="703" t="s">
+      <c r="S11" s="704"/>
+      <c r="T11" s="704"/>
+      <c r="U11" s="704" t="s">
         <v>79</v>
       </c>
-      <c r="V11" s="703"/>
-      <c r="W11" s="703"/>
+      <c r="V11" s="704"/>
+      <c r="W11" s="704"/>
       <c r="X11" s="56"/>
-      <c r="AJ11" s="703" t="s">
+      <c r="AJ11" s="704" t="s">
         <v>373</v>
       </c>
-      <c r="AK11" s="703"/>
-      <c r="AL11" s="703"/>
-      <c r="AM11" s="703"/>
+      <c r="AK11" s="704"/>
+      <c r="AL11" s="704"/>
+      <c r="AM11" s="704"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="57"/>
@@ -39520,7 +39517,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C13" s="682"/>
+      <c r="C13" s="681"/>
       <c r="D13" s="262" t="s">
         <v>407</v>
       </c>
@@ -39786,22 +39783,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A12B0C-DA54-4CAA-B658-BD043332B91F}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="B2:Y51"/>
+  <dimension ref="A2:Y51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="F1" sqref="F1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="25" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
@@ -42434,9 +42431,9 @@
   <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.9" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -42492,18 +42489,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="704" t="s">
+      <c r="E2" s="705" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="704"/>
+      <c r="F2" s="705"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="705" t="e">
+      <c r="J2" s="706" t="e">
         <f ca="1">SUMIF(O9:O100,"[",K9:K100)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="705"/>
+      <c r="K2" s="706"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -42513,10 +42510,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="706" t="s">
+      <c r="E3" s="707" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="706"/>
+      <c r="F3" s="707"/>
       <c r="G3" s="135"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -46041,7 +46038,7 @@
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.9" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -46098,18 +46095,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="704" t="s">
+      <c r="E2" s="705" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="704"/>
+      <c r="F2" s="705"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="705" t="e">
+      <c r="J2" s="706" t="e">
         <f ca="1">SUMIF(O9:O235,"[",K9:K235)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="705"/>
+      <c r="K2" s="706"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -46119,10 +46116,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="706" t="s">
+      <c r="E3" s="707" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="706"/>
+      <c r="F3" s="707"/>
       <c r="G3" s="201"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -46382,7 +46379,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="707"/>
+      <c r="A14" s="708"/>
       <c r="B14" s="51"/>
       <c r="C14" s="7"/>
       <c r="D14" s="101"/>
@@ -46416,7 +46413,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="707"/>
+      <c r="A15" s="708"/>
       <c r="B15" s="51"/>
       <c r="C15" s="7"/>
       <c r="D15" s="101"/>
@@ -54442,7 +54439,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43326.474299305555</v>
+        <v>43327.344405324075</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>

</xml_diff>

<commit_message>
fixed major issues in code & template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAjoku\Documents\GitHub\GCGRrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F2E56D-7C30-44A7-A791-8901C081C1A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A141D-7B31-4F2B-A08D-9E00303D47B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="7020" xr2:uid="{2E80CA58-8610-40E9-A54D-09997D7EA2F4}"/>
   </bookViews>
@@ -35,6 +35,7 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="\\\temp" localSheetId="6">'GCs Detail'!$E$10:$J$19,'GCs Detail'!$E$22:$J$22,'GCs Detail'!$E$26:$J$29,'GCs Detail'!$E$32:$J$43,'GCs Detail'!$E$46:$J$56,'GCs Detail'!$E$59:$J$69,'GCs Detail'!$E$72:$J$72,'GCs Detail'!$E$75:$J$75,'GCs Detail'!$E$78:$J$78,'GCs Detail'!$E$81:$J$82,'GCs Detail'!$E$85:$J$87,'GCs Detail'!$E$90:$J$96</definedName>
@@ -66,7 +67,7 @@
     <definedName name="\c_desc" localSheetId="3">'Labor Gantt'!$B$1</definedName>
     <definedName name="\c_durEND" localSheetId="2">'Staff Detail'!$O$1</definedName>
     <definedName name="\c_durSTART" localSheetId="2">'Staff Detail'!$N$1</definedName>
-    <definedName name="\c_editStart" localSheetId="4">'Non-Staff Labor'!$O$1</definedName>
+    <definedName name="\c_editStart" localSheetId="4">'Non-Staff Labor'!$L$1</definedName>
     <definedName name="\c_endcol" localSheetId="3">'Labor Gantt'!$CP$7</definedName>
     <definedName name="\c_gdur" localSheetId="3">'Labor Gantt'!$E$1</definedName>
     <definedName name="\c_group" localSheetId="6">'GCs Detail'!$O$1</definedName>
@@ -224,7 +225,7 @@
     <definedName name="\r_bin" localSheetId="9">'GRs Owner'!$A$243:$A$245</definedName>
     <definedName name="\r_blank" localSheetId="8">'GCs Owner'!$A$116</definedName>
     <definedName name="\r_blank" localSheetId="9">'GRs Owner'!$A$242</definedName>
-    <definedName name="\r_carry" localSheetId="4">'Non-Staff Labor'!#REF!</definedName>
+    <definedName name="\r_carry" localSheetId="4">'Non-Staff Labor'!$A$15</definedName>
     <definedName name="\r_constr" localSheetId="2">'Staff Detail'!$A$15</definedName>
     <definedName name="\r_dates" localSheetId="3">'Labor Gantt'!$A$1</definedName>
     <definedName name="\r_defaultEnd" localSheetId="8">'GCs Owner'!$A$125</definedName>
@@ -389,7 +390,7 @@
     <definedName name="staffcounter">Settings!$H$22</definedName>
     <definedName name="testg">Code!$J$8</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcMode="manual"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6089,7 +6090,7 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="709">
+  <cellXfs count="710">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -8127,11 +8128,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="77" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -8392,7 +8396,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>593800</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
@@ -8446,7 +8450,7 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[5]!onopen" textlink="">
+    <xdr:sp macro="[6]!onopen" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
@@ -8605,7 +8609,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>187000</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!lessMONTHdetailCLICK">
+    <xdr:pic macro="[4]!lessMONTHdetailCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="\\lessMONTHdetail">
           <a:extLst>
@@ -8655,7 +8659,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>167879</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!plusCLICK">
+    <xdr:pic macro="[4]!plusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="\\Plus">
           <a:extLst>
@@ -8705,7 +8709,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>167879</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!minusCLICK">
+    <xdr:pic macro="[4]!minusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="\\Minus">
           <a:extLst>
@@ -8755,7 +8759,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>187000</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!lessRATEdetailCLICK">
+    <xdr:pic macro="[4]!lessRATEdetailCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="15" name="\\lessRATEdetail">
           <a:extLst>
@@ -8805,7 +8809,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
@@ -8855,7 +8859,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>190585</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!moreMONTHdetailCLICK">
+    <xdr:pic macro="[4]!moreMONTHdetailCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="599" name="\\moreMONTHdetail">
           <a:extLst>
@@ -8905,7 +8909,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>190585</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!moreRATEdetailCLICK">
+    <xdr:pic macro="[4]!moreRATEdetailCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="280" name="\\moreRATEdetail">
           <a:extLst>
@@ -8955,7 +8959,7 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>225744</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!precon_listMENU_CLICK">
+    <xdr:pic macro="[4]!precon_listMENU_CLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="627" name="Picture 626">
           <a:extLst>
@@ -9005,7 +9009,7 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>225745</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!con_listMENU_CLICK">
+    <xdr:pic macro="[4]!con_listMENU_CLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="342" name="Picture 341">
           <a:extLst>
@@ -9055,7 +9059,7 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>18678</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!MakeChart">
+    <xdr:pic macro="[4]!MakeChart">
       <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="Graphic 21" descr="Bar chart" hidden="1">
           <a:extLst>
@@ -9108,7 +9112,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>510541</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
@@ -9146,7 +9150,7 @@
       <xdr:rowOff>44770</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="886967" cy="182880"/>
-    <xdr:pic macro="[3]!phase_listMENU_CLICK">
+    <xdr:pic macro="[4]!phase_listMENU_CLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="62" name="\phasestaff" hidden="1">
           <a:extLst>
@@ -9196,7 +9200,7 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>99058</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!addPhase_Click">
+    <xdr:pic macro="[4]!addPhase_Click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2070" name="Picture 2069">
           <a:extLst>
@@ -9251,7 +9255,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>34694</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
@@ -9301,7 +9305,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>25804</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="[3]!dummy" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 5">
           <a:extLst>
@@ -9464,7 +9468,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
@@ -9514,7 +9518,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>3649</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[4]!addITEM_Click">
+    <xdr:pic macro="[5]!addITEM_Click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="\addItem" hidden="1">
           <a:extLst>
@@ -9564,7 +9568,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>187072</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[4]!addTemp_Click">
+    <xdr:pic macro="[5]!addTemp_Click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="\addtemp">
           <a:extLst>
@@ -9614,7 +9618,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>26967</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="[3]!dummy" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="TextBox 3">
           <a:extLst>
@@ -9772,7 +9776,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="\\more01" hidden="1">
           <a:extLst>
@@ -9817,7 +9821,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="\\less01">
           <a:extLst>
@@ -9862,7 +9866,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="\\more02" hidden="1">
           <a:extLst>
@@ -9907,7 +9911,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="\\less02">
           <a:extLst>
@@ -9952,7 +9956,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="\\more03" hidden="1">
           <a:extLst>
@@ -9997,7 +10001,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="\\less03">
           <a:extLst>
@@ -10042,7 +10046,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="\\more04" hidden="1">
           <a:extLst>
@@ -10087,7 +10091,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="\\less04">
           <a:extLst>
@@ -10132,7 +10136,7 @@
       <xdr:rowOff>22496</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="259808"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="\\more05" hidden="1">
           <a:extLst>
@@ -10177,7 +10181,7 @@
       <xdr:rowOff>20151</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="264497"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="\\less05">
           <a:extLst>
@@ -10222,7 +10226,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="12" name="\\more06" hidden="1">
           <a:extLst>
@@ -10267,7 +10271,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="\\less06">
           <a:extLst>
@@ -10312,7 +10316,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="14" name="\\more07" hidden="1">
           <a:extLst>
@@ -10357,7 +10361,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="15" name="\\less07">
           <a:extLst>
@@ -10402,7 +10406,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="16" name="\\more08" hidden="1">
           <a:extLst>
@@ -10447,7 +10451,7 @@
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="17" name="\\less08">
           <a:extLst>
@@ -10492,7 +10496,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="18" name="\\more09" hidden="1">
           <a:extLst>
@@ -10537,7 +10541,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="19" name="\\less09">
           <a:extLst>
@@ -10582,7 +10586,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="20" name="\\more10" hidden="1">
           <a:extLst>
@@ -10627,7 +10631,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="21" name="\\less10">
           <a:extLst>
@@ -10672,7 +10676,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="\\more11" hidden="1">
           <a:extLst>
@@ -10717,7 +10721,7 @@
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="23" name="\\less11">
           <a:extLst>
@@ -10762,7 +10766,7 @@
       <xdr:rowOff>17586</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="24" name="\\more12" hidden="1">
           <a:extLst>
@@ -10807,7 +10811,7 @@
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="25" name="\\less12">
           <a:extLst>
@@ -10852,7 +10856,7 @@
       <xdr:rowOff>62753</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1998321" cy="617780"/>
-    <xdr:pic macro="[3]!toggleADMINmode">
+    <xdr:pic macro="[4]!toggleADMINmode">
       <xdr:nvPicPr>
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
@@ -10897,7 +10901,7 @@
       <xdr:rowOff>169080</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3913430" cy="404566"/>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="27" name="Picture 26">
           <a:extLst>
@@ -10946,7 +10950,7 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>230123</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!addtrailer_CLICK">
+    <xdr:pic macro="[4]!addtrailer_CLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
@@ -10996,7 +11000,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>326952</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
@@ -11046,7 +11050,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>244378</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!plusCLICK">
+    <xdr:pic macro="[4]!plusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="30" name="\\Plus">
           <a:extLst>
@@ -11096,7 +11100,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>244938</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!minusCLICK">
+    <xdr:pic macro="[4]!minusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="31" name="\\Minus" hidden="1">
           <a:extLst>
@@ -11146,7 +11150,7 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>223896</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="32" name="\m\carry" hidden="1">
           <a:extLst>
@@ -11191,7 +11195,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="244475" cy="251517"/>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="33" name="\m\burger" hidden="1">
           <a:extLst>
@@ -11317,7 +11321,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19223</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="35" name="\m\x" hidden="1">
           <a:extLst>
@@ -11669,7 +11673,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="41" name="\c\minus_\" hidden="1">
           <a:extLst>
@@ -11737,7 +11741,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="42" name="\c\catch_\" hidden="1">
           <a:extLst>
@@ -11805,7 +11809,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="43" name="\c\prorata_\" hidden="1">
           <a:extLst>
@@ -11873,7 +11877,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>133542</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="44" name="\s\ready" hidden="1">
           <a:extLst>
@@ -11923,7 +11927,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>98211</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="45" name="\s\sync" hidden="1">
           <a:extLst>
@@ -11973,7 +11977,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="\\more01" hidden="1">
           <a:extLst>
@@ -12018,7 +12022,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="\\less01">
           <a:extLst>
@@ -12063,7 +12067,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="\\more02" hidden="1">
           <a:extLst>
@@ -12108,7 +12112,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="\\less02">
           <a:extLst>
@@ -12153,7 +12157,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="\\more03" hidden="1">
           <a:extLst>
@@ -12198,7 +12202,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="\\less03">
           <a:extLst>
@@ -12243,7 +12247,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="\\more04" hidden="1">
           <a:extLst>
@@ -12288,7 +12292,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="\\less04">
           <a:extLst>
@@ -12333,7 +12337,7 @@
       <xdr:rowOff>22496</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="259808"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="\\more05" hidden="1">
           <a:extLst>
@@ -12378,7 +12382,7 @@
       <xdr:rowOff>20151</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="264497"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="\\less05">
           <a:extLst>
@@ -12423,7 +12427,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="12" name="\\more06" hidden="1">
           <a:extLst>
@@ -12468,7 +12472,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="13" name="\\less06">
           <a:extLst>
@@ -12513,7 +12517,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="14" name="\\more07" hidden="1">
           <a:extLst>
@@ -12558,7 +12562,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="15" name="\\less07">
           <a:extLst>
@@ -12603,7 +12607,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="16" name="\\more08" hidden="1">
           <a:extLst>
@@ -12648,7 +12652,7 @@
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="17" name="\\less08">
           <a:extLst>
@@ -12693,7 +12697,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="18" name="\\more09" hidden="1">
           <a:extLst>
@@ -12738,7 +12742,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="19" name="\\less09">
           <a:extLst>
@@ -12783,7 +12787,7 @@
       <xdr:rowOff>17584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="20" name="\\more10" hidden="1">
           <a:extLst>
@@ -12828,7 +12832,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="21" name="\\less10">
           <a:extLst>
@@ -12873,7 +12877,7 @@
       <xdr:rowOff>17585</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="\\more11" hidden="1">
           <a:extLst>
@@ -12918,7 +12922,7 @@
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="23" name="\\less11">
           <a:extLst>
@@ -12963,7 +12967,7 @@
       <xdr:rowOff>62753</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1998321" cy="617780"/>
-    <xdr:pic macro="[3]!toggleADMINmode">
+    <xdr:pic macro="[4]!toggleADMINmode">
       <xdr:nvPicPr>
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
@@ -13013,7 +13017,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>338382</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
@@ -13063,7 +13067,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>263428</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!plusCLICK">
+    <xdr:pic macro="[4]!plusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="30" name="\\Plus">
           <a:extLst>
@@ -13113,7 +13117,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>262083</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!minusCLICK">
+    <xdr:pic macro="[4]!minusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="31" name="\\Minus" hidden="1">
           <a:extLst>
@@ -13163,7 +13167,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>187419</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="32" name="\m\carry" hidden="1">
           <a:extLst>
@@ -13208,7 +13212,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="246380" cy="253481"/>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="33" name="\m\burger" hidden="1">
           <a:extLst>
@@ -13334,7 +13338,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>187619</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="35" name="\m\x" hidden="1">
           <a:extLst>
@@ -13686,7 +13690,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="41" name="\c\minus_\" hidden="1">
           <a:extLst>
@@ -13754,7 +13758,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="42" name="\c\catch_\" hidden="1">
           <a:extLst>
@@ -13822,7 +13826,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="43" name="\c\prorata_\" hidden="1">
           <a:extLst>
@@ -13890,7 +13894,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>148782</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="44" name="\s\ready" hidden="1">
           <a:extLst>
@@ -13940,7 +13944,7 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>109641</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="45" name="\s\sync" hidden="1">
           <a:extLst>
@@ -13990,7 +13994,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>33826</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="46" name="Picture 45">
           <a:extLst>
@@ -14028,7 +14032,7 @@
       <xdr:rowOff>17586</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="49" name="\\more12" hidden="1">
           <a:extLst>
@@ -14073,7 +14077,7 @@
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="50" name="\\less12">
           <a:extLst>
@@ -14118,7 +14122,7 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="72" name="\\more14" hidden="1">
           <a:extLst>
@@ -14163,7 +14167,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="75" name="\\more17" hidden="1">
           <a:extLst>
@@ -14208,7 +14212,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="76" name="\\more18" hidden="1">
           <a:extLst>
@@ -14253,7 +14257,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="77" name="\\more19" hidden="1">
           <a:extLst>
@@ -14298,7 +14302,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="78" name="\\more20" hidden="1">
           <a:extLst>
@@ -14343,7 +14347,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="79" name="\\more21" hidden="1">
           <a:extLst>
@@ -14388,7 +14392,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="82" name="\\less14">
           <a:extLst>
@@ -14433,7 +14437,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="85" name="\\less17">
           <a:extLst>
@@ -14478,7 +14482,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="86" name="\\less18">
           <a:extLst>
@@ -14523,7 +14527,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="87" name="\\less19">
           <a:extLst>
@@ -14568,7 +14572,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="88" name="\\less20">
           <a:extLst>
@@ -14613,7 +14617,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="89" name="\\less21">
           <a:extLst>
@@ -14658,7 +14662,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="66" name="\\less21" hidden="1">
           <a:extLst>
@@ -14703,7 +14707,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="67" name="\\more22" hidden="1">
           <a:extLst>
@@ -14748,7 +14752,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="68" name="\\less22">
           <a:extLst>
@@ -14793,7 +14797,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270525" cy="269631"/>
-    <xdr:pic macro="[3]!more_click">
+    <xdr:pic macro="[4]!more_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="60" name="\\more15" hidden="1">
           <a:extLst>
@@ -14838,7 +14842,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="279661" cy="274320"/>
-    <xdr:pic macro="[3]!less_click">
+    <xdr:pic macro="[4]!less_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="61" name="\\less15">
           <a:extLst>
@@ -14893,7 +14897,7 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>284081</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
@@ -14943,7 +14947,7 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>184337</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!dummy" textlink="">
+    <xdr:sp macro="[4]!dummy" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="41" name="\c_line" hidden="1">
           <a:extLst>
@@ -15014,7 +15018,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>291757</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="\c_main" hidden="1">
           <a:extLst>
@@ -15820,7 +15824,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="\c\H_\" hidden="1">
           <a:extLst>
@@ -15888,7 +15892,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="\c\a_\" hidden="1">
           <a:extLst>
@@ -15956,7 +15960,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="18" name="\c\plus_\" hidden="1">
           <a:extLst>
@@ -16024,7 +16028,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="\c\arrow_\" hidden="1">
           <a:extLst>
@@ -16092,7 +16096,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="\c\updown_\" hidden="1">
           <a:extLst>
@@ -16160,7 +16164,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>250452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="21" name="\c\minus_\" hidden="1">
           <a:extLst>
@@ -16228,7 +16232,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>291757</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="\c_x" hidden="1">
           <a:extLst>
@@ -16378,7 +16382,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>17556</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
@@ -16428,7 +16432,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>168824</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!minusCLICK">
+    <xdr:pic macro="[4]!minusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="27" name="\\Minus" hidden="1">
           <a:extLst>
@@ -16478,7 +16482,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>171513</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!plusCLICK">
+    <xdr:pic macro="[4]!plusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="28" name="\\Plus">
           <a:extLst>
@@ -16528,7 +16532,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!restoreDETAIL" textlink="">
+    <xdr:sp macro="[4]!restoreDETAIL" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="29" name="\N\1" hidden="1">
           <a:extLst>
@@ -16601,7 +16605,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!N2_Click" textlink="">
+    <xdr:sp macro="[4]!N2_Click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="30" name="\N\2" hidden="1">
           <a:extLst>
@@ -16867,7 +16871,7 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>287891</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
+    <xdr:pic macro="[3]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
@@ -16917,7 +16921,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>283039</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="\c_main" hidden="1">
           <a:extLst>
@@ -17723,7 +17727,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="\c\H_\" hidden="1">
           <a:extLst>
@@ -17791,7 +17795,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="\c\a_\" hidden="1">
           <a:extLst>
@@ -17859,7 +17863,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="18" name="\c\plus_\" hidden="1">
           <a:extLst>
@@ -17927,7 +17931,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="19" name="\c\arrow_\" hidden="1">
           <a:extLst>
@@ -17995,7 +17999,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="\c\updown_\" hidden="1">
           <a:extLst>
@@ -18063,7 +18067,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>243728</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!context_click" textlink="">
+    <xdr:sp macro="[4]!context_click" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="21" name="\c\minus_\" hidden="1">
           <a:extLst>
@@ -18131,7 +18135,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>283039</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!context_click">
+    <xdr:pic macro="[4]!context_click">
       <xdr:nvPicPr>
         <xdr:cNvPr id="22" name="\c_x" hidden="1">
           <a:extLst>
@@ -18281,7 +18285,7 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!dummy" textlink="">
+    <xdr:sp macro="[4]!dummy" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="25" name="\c_line" hidden="1">
           <a:extLst>
@@ -18352,7 +18356,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>21366</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!dummy">
+    <xdr:pic macro="[4]!dummy">
       <xdr:nvPicPr>
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
@@ -18402,7 +18406,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>168824</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!minusCLICK">
+    <xdr:pic macro="[4]!minusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="27" name="\\Minus" hidden="1">
           <a:extLst>
@@ -18452,7 +18456,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>169608</xdr:rowOff>
     </xdr:to>
-    <xdr:pic macro="[3]!plusCLICK">
+    <xdr:pic macro="[4]!plusCLICK">
       <xdr:nvPicPr>
         <xdr:cNvPr id="28" name="\\Plus">
           <a:extLst>
@@ -18502,7 +18506,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="[3]!restoreDETAIL" textlink="">
+    <xdr:sp macro="[4]!restoreDETAIL" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="29" name="\N\1" hidden="1">
           <a:extLst>
@@ -19811,6 +19815,52 @@
       <sheetName val="GCs Owner"/>
       <sheetName val="GRs Owner"/>
       <sheetName val="Bin"/>
+      <sheetName val="meta"/>
+      <sheetName val="Errors"/>
+      <sheetName val="Code"/>
+      <sheetName val="CostCodes"/>
+      <sheetName val="splash"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="dummy"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Settings"/>
+      <sheetName val="Staff Detail"/>
+      <sheetName val="LaborOLD"/>
+      <sheetName val="Labor Gantt"/>
+      <sheetName val="Non-Staff Labor"/>
+      <sheetName val="Rate Tables"/>
+      <sheetName val="GCs Detail"/>
+      <sheetName val="GRs Detail"/>
+      <sheetName val="GCs Owner"/>
+      <sheetName val="GRs Owner"/>
+      <sheetName val="Bin"/>
       <sheetName val="Errors"/>
       <sheetName val="Code"/>
       <sheetName val="CostCodes"/>
@@ -19860,7 +19910,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -19937,7 +19987,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -20359,8 +20409,8 @@
       <c r="C4" s="314" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="686"/>
-      <c r="E4" s="687"/>
+      <c r="D4" s="687"/>
+      <c r="E4" s="688"/>
       <c r="F4" s="315"/>
       <c r="G4" s="314" t="s">
         <v>207</v>
@@ -20387,8 +20437,8 @@
       <c r="C5" s="314" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="686"/>
-      <c r="E5" s="687"/>
+      <c r="D5" s="687"/>
+      <c r="E5" s="688"/>
       <c r="F5" s="315"/>
       <c r="G5" s="314" t="s">
         <v>208</v>
@@ -20415,10 +20465,10 @@
       <c r="C6" s="314" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="686" t="s">
+      <c r="D6" s="687" t="s">
         <v>274</v>
       </c>
-      <c r="E6" s="687"/>
+      <c r="E6" s="688"/>
       <c r="F6" s="315"/>
       <c r="G6" s="314" t="s">
         <v>9</v>
@@ -20428,7 +20478,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I6" s="315"/>
-      <c r="J6" s="688" t="s">
+      <c r="J6" s="689" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="514" t="e">
@@ -20451,10 +20501,10 @@
       <c r="C7" s="314" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="684" t="s">
+      <c r="D7" s="685" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="685"/>
+      <c r="E7" s="686"/>
       <c r="F7" s="315"/>
       <c r="G7" s="315"/>
       <c r="H7" s="515" t="e">
@@ -20462,7 +20512,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="688"/>
+      <c r="J7" s="689"/>
       <c r="K7" s="515" t="e">
         <f ca="1">IF(cDateDiff("WW",\cstart,\cend)&gt;0,cDateDiff("WW",\cstart,\cend),0)</f>
         <v>#NAME?</v>
@@ -20554,7 +20604,7 @@
       </c>
       <c r="D11" s="12">
         <f ca="1">NOW()</f>
-        <v>43327.35778726852</v>
+        <v>43333.416436111111</v>
       </c>
       <c r="E11" s="315"/>
       <c r="F11" s="313"/>
@@ -20672,10 +20722,10 @@
       <c r="C16" s="314" t="s">
         <v>227</v>
       </c>
-      <c r="D16" s="686" t="s">
+      <c r="D16" s="687" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="687"/>
+      <c r="E16" s="688"/>
       <c r="F16" s="315"/>
       <c r="G16" s="314" t="s">
         <v>226</v>
@@ -20931,7 +20981,7 @@
   <dimension ref="A1:N1074"/>
   <sheetViews>
     <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -21050,7 +21100,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43327.35778726852</v>
+        <v>43333.416436111111</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>
@@ -34479,12 +34529,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F093129-0C35-4C29-B2A0-FFC991FE5B09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1A4F89-FC04-4A38-97E9-6714BC2884DC}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34494,7 +34544,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -34515,7 +34565,7 @@
     <sheetView showZeros="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="12" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4:E4"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -34578,11 +34628,11 @@
       <c r="AM1" s="321"/>
     </row>
     <row r="2" spans="1:43" s="311" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="689" t="str">
+      <c r="B2" s="690" t="str">
         <f>IF(Settings!D4&lt;&gt;0,Settings!D4,"")</f>
         <v/>
       </c>
-      <c r="C2" s="689"/>
+      <c r="C2" s="690"/>
       <c r="D2" s="324"/>
       <c r="G2" s="325"/>
       <c r="AB2" s="326"/>
@@ -34594,15 +34644,15 @@
       <c r="AQ2" s="321"/>
     </row>
     <row r="3" spans="1:43" s="311" customFormat="1" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="690" t="str">
+      <c r="B3" s="691" t="str">
         <f>IF(Settings!D5&lt;&gt;0,Settings!D5,"")</f>
         <v/>
       </c>
-      <c r="C3" s="690"/>
+      <c r="C3" s="691"/>
       <c r="D3" s="327"/>
       <c r="E3" s="328">
         <f ca="1">Settings!\date</f>
-        <v>43327.35778726852</v>
+        <v>43333.416436111111</v>
       </c>
       <c r="Q3" s="326"/>
       <c r="AD3" s="326"/>
@@ -34829,18 +34879,18 @@
       <c r="B11" s="351"/>
       <c r="C11" s="352"/>
       <c r="D11" s="352"/>
-      <c r="E11" s="693" t="s">
+      <c r="E11" s="694" t="s">
         <v>245</v>
       </c>
       <c r="F11" s="352"/>
-      <c r="G11" s="693" t="s">
+      <c r="G11" s="694" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="352"/>
-      <c r="I11" s="693" t="s">
+      <c r="I11" s="694" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="693" t="s">
+      <c r="J11" s="694" t="s">
         <v>246</v>
       </c>
       <c r="K11" s="353"/>
@@ -34852,40 +34902,40 @@
       </c>
       <c r="O11" s="359"/>
       <c r="P11" s="360"/>
-      <c r="Q11" s="695" t="s">
+      <c r="Q11" s="696" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="699" t="s">
+      <c r="R11" s="700" t="s">
         <v>368</v>
       </c>
-      <c r="S11" s="697" t="s">
+      <c r="S11" s="698" t="s">
         <v>369</v>
       </c>
-      <c r="T11" s="691" t="s">
+      <c r="T11" s="692" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="691" t="s">
+      <c r="U11" s="692" t="s">
         <v>234</v>
       </c>
-      <c r="V11" s="691" t="s">
+      <c r="V11" s="692" t="s">
         <v>235</v>
       </c>
-      <c r="W11" s="691" t="s">
+      <c r="W11" s="692" t="s">
         <v>239</v>
       </c>
-      <c r="X11" s="691" t="s">
+      <c r="X11" s="692" t="s">
         <v>237</v>
       </c>
-      <c r="Y11" s="691" t="s">
+      <c r="Y11" s="692" t="s">
         <v>238</v>
       </c>
-      <c r="Z11" s="691" t="s">
+      <c r="Z11" s="692" t="s">
         <v>241</v>
       </c>
-      <c r="AA11" s="691" t="s">
+      <c r="AA11" s="692" t="s">
         <v>240</v>
       </c>
-      <c r="AB11" s="691" t="s">
+      <c r="AB11" s="692" t="s">
         <v>236</v>
       </c>
       <c r="AC11" s="361"/>
@@ -34909,14 +34959,14 @@
       <c r="D12" s="365" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="694"/>
+      <c r="E12" s="695"/>
       <c r="F12" s="365"/>
-      <c r="G12" s="694"/>
+      <c r="G12" s="695"/>
       <c r="H12" s="365" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="694"/>
-      <c r="J12" s="694"/>
+      <c r="I12" s="695"/>
+      <c r="J12" s="695"/>
       <c r="K12" s="366" t="s">
         <v>232</v>
       </c>
@@ -34931,18 +34981,18 @@
       <c r="P12" s="373" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="696"/>
-      <c r="R12" s="700"/>
-      <c r="S12" s="698"/>
-      <c r="T12" s="692"/>
-      <c r="U12" s="692"/>
-      <c r="V12" s="692"/>
-      <c r="W12" s="692"/>
-      <c r="X12" s="692"/>
-      <c r="Y12" s="692"/>
-      <c r="Z12" s="692"/>
-      <c r="AA12" s="692"/>
-      <c r="AB12" s="692"/>
+      <c r="Q12" s="697"/>
+      <c r="R12" s="701"/>
+      <c r="S12" s="699"/>
+      <c r="T12" s="693"/>
+      <c r="U12" s="693"/>
+      <c r="V12" s="693"/>
+      <c r="W12" s="693"/>
+      <c r="X12" s="693"/>
+      <c r="Y12" s="693"/>
+      <c r="Z12" s="693"/>
+      <c r="AA12" s="693"/>
+      <c r="AB12" s="693"/>
       <c r="AC12" s="374"/>
       <c r="AD12" s="375" t="s">
         <v>2</v>
@@ -37535,22 +37585,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="I1" s="701"/>
-      <c r="J1" s="701"/>
-      <c r="K1" s="701"/>
-      <c r="L1" s="701"/>
-      <c r="M1" s="701"/>
-      <c r="N1" s="701"/>
-      <c r="O1" s="701"/>
-      <c r="P1" s="701"/>
-      <c r="Q1" s="701"/>
-      <c r="R1" s="701"/>
-      <c r="S1" s="701"/>
-      <c r="T1" s="701"/>
-      <c r="U1" s="701"/>
-      <c r="V1" s="701"/>
-      <c r="W1" s="701"/>
-      <c r="X1" s="701"/>
+      <c r="I1" s="702"/>
+      <c r="J1" s="702"/>
+      <c r="K1" s="702"/>
+      <c r="L1" s="702"/>
+      <c r="M1" s="702"/>
+      <c r="N1" s="702"/>
+      <c r="O1" s="702"/>
+      <c r="P1" s="702"/>
+      <c r="Q1" s="702"/>
+      <c r="R1" s="702"/>
+      <c r="S1" s="702"/>
+      <c r="T1" s="702"/>
+      <c r="U1" s="702"/>
+      <c r="V1" s="702"/>
+      <c r="W1" s="702"/>
+      <c r="X1" s="702"/>
       <c r="Y1" s="608"/>
       <c r="Z1" s="608"/>
       <c r="AA1" s="608"/>
@@ -38051,7 +38101,7 @@
       <c r="CL8" s="634"/>
       <c r="CM8" s="634"/>
       <c r="CN8" s="634"/>
-      <c r="CO8" s="639"/>
+      <c r="CO8" s="634"/>
       <c r="CP8" s="623"/>
       <c r="CR8" s="634"/>
     </row>
@@ -38274,7 +38324,7 @@
       </c>
       <c r="G11" s="651"/>
       <c r="H11" s="652"/>
-      <c r="I11" s="682"/>
+      <c r="I11" s="683"/>
       <c r="J11" s="607"/>
       <c r="K11" s="607"/>
       <c r="L11" s="607"/>
@@ -38358,9 +38408,9 @@
       <c r="CL11" s="607"/>
       <c r="CM11" s="607"/>
       <c r="CN11" s="607"/>
-      <c r="CO11" s="683"/>
+      <c r="CO11" s="684"/>
       <c r="CP11" s="623"/>
-      <c r="CR11" s="607"/>
+      <c r="CR11" s="681"/>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="B12" s="606"/>
@@ -39344,7 +39394,7 @@
   <dimension ref="A1:AM19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39382,13 +39432,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="U1" s="702"/>
-      <c r="V1" s="702"/>
-      <c r="W1" s="702"/>
-      <c r="AJ1" s="702"/>
-      <c r="AK1" s="702"/>
-      <c r="AL1" s="702"/>
-      <c r="AM1" s="702"/>
+      <c r="U1" s="703"/>
+      <c r="V1" s="703"/>
+      <c r="W1" s="703"/>
+      <c r="AJ1" s="703"/>
+      <c r="AK1" s="703"/>
+      <c r="AL1" s="703"/>
+      <c r="AM1" s="703"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="H6" s="672"/>
@@ -39402,43 +39452,43 @@
       <c r="C11" s="57"/>
       <c r="D11" s="264"/>
       <c r="E11" s="265"/>
-      <c r="F11" s="703" t="s">
+      <c r="F11" s="704" t="s">
         <v>1009</v>
       </c>
-      <c r="G11" s="703"/>
-      <c r="H11" s="703"/>
-      <c r="I11" s="704" t="s">
+      <c r="G11" s="704"/>
+      <c r="H11" s="704"/>
+      <c r="I11" s="705" t="s">
         <v>470</v>
       </c>
-      <c r="J11" s="704"/>
-      <c r="K11" s="704"/>
-      <c r="L11" s="704" t="s">
+      <c r="J11" s="705"/>
+      <c r="K11" s="705"/>
+      <c r="L11" s="705" t="s">
         <v>364</v>
       </c>
-      <c r="M11" s="704"/>
-      <c r="N11" s="704"/>
-      <c r="O11" s="704" t="s">
+      <c r="M11" s="705"/>
+      <c r="N11" s="705"/>
+      <c r="O11" s="705" t="s">
         <v>1010</v>
       </c>
-      <c r="P11" s="704"/>
-      <c r="Q11" s="704"/>
-      <c r="R11" s="704" t="s">
+      <c r="P11" s="705"/>
+      <c r="Q11" s="705"/>
+      <c r="R11" s="705" t="s">
         <v>1011</v>
       </c>
-      <c r="S11" s="704"/>
-      <c r="T11" s="704"/>
-      <c r="U11" s="704" t="s">
+      <c r="S11" s="705"/>
+      <c r="T11" s="705"/>
+      <c r="U11" s="705" t="s">
         <v>79</v>
       </c>
-      <c r="V11" s="704"/>
-      <c r="W11" s="704"/>
+      <c r="V11" s="705"/>
+      <c r="W11" s="705"/>
       <c r="X11" s="56"/>
-      <c r="AJ11" s="704" t="s">
+      <c r="AJ11" s="705" t="s">
         <v>373</v>
       </c>
-      <c r="AK11" s="704"/>
-      <c r="AL11" s="704"/>
-      <c r="AM11" s="704"/>
+      <c r="AK11" s="705"/>
+      <c r="AL11" s="705"/>
+      <c r="AM11" s="705"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="57"/>
@@ -39517,7 +39567,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C13" s="681"/>
+      <c r="C13" s="682"/>
       <c r="D13" s="262" t="s">
         <v>407</v>
       </c>
@@ -42431,9 +42481,9 @@
   <dimension ref="A1:T129"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.9" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -42489,18 +42539,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="705" t="s">
+      <c r="E2" s="706" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="705"/>
+      <c r="F2" s="706"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="706" t="e">
+      <c r="J2" s="707" t="e">
         <f ca="1">SUMIF(O9:O100,"[",K9:K100)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="706"/>
+      <c r="K2" s="707"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -42510,10 +42560,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="707" t="s">
+      <c r="E3" s="708" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="707"/>
+      <c r="F3" s="708"/>
       <c r="G3" s="135"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -43090,10 +43140,7 @@
       <c r="L22" s="38"/>
       <c r="M22" s="104"/>
       <c r="N22" s="105"/>
-      <c r="O22" s="106">
-        <f t="shared" ref="O22" si="4">OR(NOT(ISERROR(SEARCH($F$5,Q22))),Q22=0)*OR(NOT(ISERROR(SEARCH($F$6,R22))),R22=0)</f>
-        <v>1</v>
-      </c>
+      <c r="O22" s="106"/>
       <c r="P22" s="106"/>
       <c r="Q22" s="108"/>
       <c r="R22" s="108"/>
@@ -43370,14 +43417,14 @@
         <v>500</v>
       </c>
       <c r="K32" s="150">
-        <f t="shared" ref="K32:K43" si="5">SUM(H32*J32)</f>
+        <f t="shared" ref="K32:K43" si="4">SUM(H32*J32)</f>
         <v>0</v>
       </c>
       <c r="L32" s="38"/>
       <c r="M32" s="104"/>
       <c r="N32" s="105"/>
       <c r="O32" s="106">
-        <f t="shared" ref="O32:O37" si="6">OR(NOT(ISERROR(SEARCH($F$5,Q32))),Q32=0)*OR(NOT(ISERROR(SEARCH($F$6,R32))),R32=0)</f>
+        <f t="shared" ref="O32:O37" si="5">OR(NOT(ISERROR(SEARCH($F$5,Q32))),Q32=0)*OR(NOT(ISERROR(SEARCH($F$6,R32))),R32=0)</f>
         <v>1</v>
       </c>
       <c r="P32" s="106"/>
@@ -43407,14 +43454,14 @@
         <v>12000</v>
       </c>
       <c r="K33" s="152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L33" s="38"/>
       <c r="M33" s="104"/>
       <c r="N33" s="105"/>
       <c r="O33" s="106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P33" s="106"/>
@@ -43445,14 +43492,14 @@
         <v>900</v>
       </c>
       <c r="K34" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L34" s="38"/>
       <c r="M34" s="104"/>
       <c r="N34" s="105"/>
       <c r="O34" s="106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P34" s="106"/>
@@ -43482,14 +43529,14 @@
         <v>1250</v>
       </c>
       <c r="K35" s="152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L35" s="38"/>
       <c r="M35" s="104"/>
       <c r="N35" s="105"/>
       <c r="O35" s="106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P35" s="106"/>
@@ -43520,14 +43567,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K36" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L36" s="38"/>
       <c r="M36" s="104"/>
       <c r="N36" s="105"/>
       <c r="O36" s="106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P36" s="106"/>
@@ -43558,14 +43605,14 @@
         <v>500</v>
       </c>
       <c r="K37" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L37" s="38"/>
       <c r="M37" s="104"/>
       <c r="N37" s="105"/>
       <c r="O37" s="106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P37" s="106"/>
@@ -43598,14 +43645,14 @@
         <v>350</v>
       </c>
       <c r="K38" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L38" s="38"/>
       <c r="M38" s="104"/>
       <c r="N38" s="105"/>
       <c r="O38" s="106">
-        <f t="shared" ref="O38:O43" si="7">OR(NOT(ISERROR(SEARCH($F$5,Q38))),Q38=0)*OR(NOT(ISERROR(SEARCH($F$6,R38))),R38=0)</f>
+        <f t="shared" ref="O38:O43" si="6">OR(NOT(ISERROR(SEARCH($F$5,Q38))),Q38=0)*OR(NOT(ISERROR(SEARCH($F$6,R38))),R38=0)</f>
         <v>1</v>
       </c>
       <c r="P38" s="106"/>
@@ -43635,14 +43682,14 @@
         <v>600</v>
       </c>
       <c r="K39" s="152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L39" s="38"/>
       <c r="M39" s="104"/>
       <c r="N39" s="105"/>
       <c r="O39" s="106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P39" s="106"/>
@@ -43672,14 +43719,14 @@
         <v>600</v>
       </c>
       <c r="K40" s="152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L40" s="38"/>
       <c r="M40" s="104"/>
       <c r="N40" s="105"/>
       <c r="O40" s="106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P40" s="106"/>
@@ -43710,14 +43757,14 @@
         <v>200</v>
       </c>
       <c r="K41" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L41" s="38"/>
       <c r="M41" s="104"/>
       <c r="N41" s="105"/>
       <c r="O41" s="106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P41" s="106"/>
@@ -43748,14 +43795,14 @@
         <v>500</v>
       </c>
       <c r="K42" s="152" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L42" s="38"/>
       <c r="M42" s="104"/>
       <c r="N42" s="105"/>
       <c r="O42" s="106">
-        <f t="shared" ref="O42" si="8">OR(NOT(ISERROR(SEARCH($F$5,Q42))),Q42=0)*OR(NOT(ISERROR(SEARCH($F$6,R42))),R42=0)</f>
+        <f t="shared" ref="O42" si="7">OR(NOT(ISERROR(SEARCH($F$5,Q42))),Q42=0)*OR(NOT(ISERROR(SEARCH($F$6,R42))),R42=0)</f>
         <v>0</v>
       </c>
       <c r="P42" s="106"/>
@@ -43788,14 +43835,14 @@
         <v>250</v>
       </c>
       <c r="K43" s="221" t="e">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="L43" s="38"/>
       <c r="M43" s="104"/>
       <c r="N43" s="105"/>
       <c r="O43" s="106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P43" s="106"/>
@@ -43874,7 +43921,7 @@
       <c r="M46" s="104"/>
       <c r="N46" s="105"/>
       <c r="O46" s="106">
-        <f t="shared" ref="O46:O56" si="9">OR(NOT(ISERROR(SEARCH($F$5,Q46))),Q46=0)*OR(NOT(ISERROR(SEARCH($F$6,R46))),R46=0)</f>
+        <f t="shared" ref="O46:O56" si="8">OR(NOT(ISERROR(SEARCH($F$5,Q46))),Q46=0)*OR(NOT(ISERROR(SEARCH($F$6,R46))),R46=0)</f>
         <v>1</v>
       </c>
       <c r="P46" s="106"/>
@@ -43910,7 +43957,7 @@
       <c r="M47" s="104"/>
       <c r="N47" s="105"/>
       <c r="O47" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P47" s="106"/>
@@ -43940,14 +43987,14 @@
         <v>300</v>
       </c>
       <c r="K48" s="152">
-        <f t="shared" ref="K48:K55" si="10">SUM(H48*J48)</f>
+        <f t="shared" ref="K48:K55" si="9">SUM(H48*J48)</f>
         <v>0</v>
       </c>
       <c r="L48" s="38"/>
       <c r="M48" s="104"/>
       <c r="N48" s="105"/>
       <c r="O48" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P48" s="106"/>
@@ -43978,14 +44025,14 @@
         <v>265</v>
       </c>
       <c r="K49" s="152" t="e">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="9"/>
         <v>#NAME?</v>
       </c>
       <c r="L49" s="38"/>
       <c r="M49" s="104"/>
       <c r="N49" s="105"/>
       <c r="O49" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P49" s="106"/>
@@ -44015,14 +44062,14 @@
         <v>4600</v>
       </c>
       <c r="K50" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L50" s="38"/>
       <c r="M50" s="104"/>
       <c r="N50" s="105"/>
       <c r="O50" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P50" s="106"/>
@@ -44052,14 +44099,14 @@
         <v>600</v>
       </c>
       <c r="K51" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L51" s="38"/>
       <c r="M51" s="104"/>
       <c r="N51" s="105"/>
       <c r="O51" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P51" s="106"/>
@@ -44091,14 +44138,14 @@
         <v>1820</v>
       </c>
       <c r="K52" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L52" s="38"/>
       <c r="M52" s="104"/>
       <c r="N52" s="105"/>
       <c r="O52" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P52" s="106"/>
@@ -44130,14 +44177,14 @@
         <v>750</v>
       </c>
       <c r="K53" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L53" s="38"/>
       <c r="M53" s="104"/>
       <c r="N53" s="105"/>
       <c r="O53" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P53" s="106"/>
@@ -44167,14 +44214,14 @@
         <v>1200</v>
       </c>
       <c r="K54" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L54" s="38"/>
       <c r="M54" s="104"/>
       <c r="N54" s="105"/>
       <c r="O54" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P54" s="106"/>
@@ -44204,14 +44251,14 @@
         <v>50</v>
       </c>
       <c r="K55" s="152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L55" s="38"/>
       <c r="M55" s="104"/>
       <c r="N55" s="105"/>
       <c r="O55" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P55" s="106"/>
@@ -44248,7 +44295,7 @@
       <c r="M56" s="104"/>
       <c r="N56" s="105"/>
       <c r="O56" s="106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="P56" s="117"/>
@@ -44327,7 +44374,7 @@
       <c r="M59" s="104"/>
       <c r="N59" s="105"/>
       <c r="O59" s="106">
-        <f t="shared" ref="O59:O69" si="11">OR(NOT(ISERROR(SEARCH($F$5,Q59))),Q59=0)*OR(NOT(ISERROR(SEARCH($F$6,R59))),R59=0)</f>
+        <f t="shared" ref="O59:O69" si="10">OR(NOT(ISERROR(SEARCH($F$5,Q59))),Q59=0)*OR(NOT(ISERROR(SEARCH($F$6,R59))),R59=0)</f>
         <v>1</v>
       </c>
       <c r="P59" s="106"/>
@@ -44357,14 +44404,14 @@
         <v>2265</v>
       </c>
       <c r="K60" s="152">
-        <f t="shared" ref="K60:K65" si="12">SUM(H60*J60)</f>
+        <f t="shared" ref="K60:K65" si="11">SUM(H60*J60)</f>
         <v>0</v>
       </c>
       <c r="L60" s="38"/>
       <c r="M60" s="104"/>
       <c r="N60" s="105"/>
       <c r="O60" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P60" s="106"/>
@@ -44394,14 +44441,14 @@
         <v>1500</v>
       </c>
       <c r="K61" s="152">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L61" s="38"/>
       <c r="M61" s="104"/>
       <c r="N61" s="105"/>
       <c r="O61" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P61" s="106"/>
@@ -44431,14 +44478,14 @@
         <v>4500</v>
       </c>
       <c r="K62" s="152">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L62" s="38"/>
       <c r="M62" s="104"/>
       <c r="N62" s="105"/>
       <c r="O62" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P62" s="106"/>
@@ -44468,14 +44515,14 @@
         <v>150</v>
       </c>
       <c r="K63" s="152">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L63" s="38"/>
       <c r="M63" s="104"/>
       <c r="N63" s="105"/>
       <c r="O63" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P63" s="106"/>
@@ -44505,14 +44552,14 @@
         <v>150</v>
       </c>
       <c r="K64" s="152">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L64" s="38"/>
       <c r="M64" s="104"/>
       <c r="N64" s="105"/>
       <c r="O64" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P64" s="106"/>
@@ -44542,14 +44589,14 @@
         <v>450</v>
       </c>
       <c r="K65" s="152">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L65" s="38"/>
       <c r="M65" s="104"/>
       <c r="N65" s="105"/>
       <c r="O65" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P65" s="106"/>
@@ -44586,7 +44633,7 @@
       <c r="M66" s="104"/>
       <c r="N66" s="105"/>
       <c r="O66" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P66" s="106"/>
@@ -44623,7 +44670,7 @@
       <c r="M67" s="104"/>
       <c r="N67" s="105"/>
       <c r="O67" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P67" s="106"/>
@@ -44660,7 +44707,7 @@
       <c r="M68" s="104"/>
       <c r="N68" s="105"/>
       <c r="O68" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P68" s="106"/>
@@ -44697,7 +44744,7 @@
       <c r="M69" s="104"/>
       <c r="N69" s="105"/>
       <c r="O69" s="106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P69" s="106"/>
@@ -45021,7 +45068,7 @@
       <c r="M81" s="104"/>
       <c r="N81" s="105"/>
       <c r="O81" s="106">
-        <f t="shared" ref="O81:O82" si="13">OR(NOT(ISERROR(SEARCH($F$5,Q81))),Q81=0)*OR(NOT(ISERROR(SEARCH($F$6,R81))),R81=0)</f>
+        <f t="shared" ref="O81:O82" si="12">OR(NOT(ISERROR(SEARCH($F$5,Q81))),Q81=0)*OR(NOT(ISERROR(SEARCH($F$6,R81))),R81=0)</f>
         <v>1</v>
       </c>
       <c r="P81" s="106"/>
@@ -45059,7 +45106,7 @@
       <c r="M82" s="104"/>
       <c r="N82" s="105"/>
       <c r="O82" s="106">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="P82" s="106"/>
@@ -45141,7 +45188,7 @@
       <c r="M85" s="104"/>
       <c r="N85" s="105"/>
       <c r="O85" s="106">
-        <f t="shared" ref="O85:O87" si="14">OR(NOT(ISERROR(SEARCH($F$5,Q85))),Q85=0)*OR(NOT(ISERROR(SEARCH($F$6,R85))),R85=0)</f>
+        <f t="shared" ref="O85:O87" si="13">OR(NOT(ISERROR(SEARCH($F$5,Q85))),Q85=0)*OR(NOT(ISERROR(SEARCH($F$6,R85))),R85=0)</f>
         <v>1</v>
       </c>
       <c r="P85" s="106"/>
@@ -45173,14 +45220,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K86" s="173" t="e">
-        <f t="shared" ref="K86:K87" ca="1" si="15">SUM(H86*J86)</f>
+        <f t="shared" ref="K86:K87" ca="1" si="14">SUM(H86*J86)</f>
         <v>#NAME?</v>
       </c>
       <c r="L86" s="38"/>
       <c r="M86" s="104"/>
       <c r="N86" s="105"/>
       <c r="O86" s="106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="P86" s="106"/>
@@ -45211,14 +45258,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K87" s="173" t="e">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="14"/>
         <v>#NAME?</v>
       </c>
       <c r="L87" s="38"/>
       <c r="M87" s="104"/>
       <c r="N87" s="105"/>
       <c r="O87" s="106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="P87" s="106"/>
@@ -45328,14 +45375,14 @@
         <v>2000</v>
       </c>
       <c r="K91" s="150">
-        <f t="shared" ref="K91:K93" si="16">SUM(H91*J91)</f>
+        <f t="shared" ref="K91:K93" si="15">SUM(H91*J91)</f>
         <v>2000</v>
       </c>
       <c r="L91" s="38"/>
       <c r="M91" s="104"/>
       <c r="N91" s="105"/>
       <c r="O91" s="106">
-        <f t="shared" ref="O91:O92" si="17">OR(NOT(ISERROR(SEARCH($F$5,Q91))),Q91=0)*OR(NOT(ISERROR(SEARCH($F$6,R91))),R91=0)</f>
+        <f t="shared" ref="O91:O92" si="16">OR(NOT(ISERROR(SEARCH($F$5,Q91))),Q91=0)*OR(NOT(ISERROR(SEARCH($F$6,R91))),R91=0)</f>
         <v>1</v>
       </c>
       <c r="P91" s="106"/>
@@ -45365,14 +45412,14 @@
         <v>0</v>
       </c>
       <c r="K92" s="150">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L92" s="38"/>
       <c r="M92" s="104"/>
       <c r="N92" s="105"/>
       <c r="O92" s="106">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P92" s="106"/>
@@ -45404,14 +45451,14 @@
         <v>0</v>
       </c>
       <c r="K93" s="150">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L93" s="38"/>
       <c r="M93" s="104"/>
       <c r="N93" s="105"/>
       <c r="O93" s="106">
-        <f t="shared" ref="O93" si="18">OR(NOT(ISERROR(SEARCH($F$5,Q93))),Q93=0)*OR(NOT(ISERROR(SEARCH($F$6,R93))),R93=0)</f>
+        <f t="shared" ref="O93" si="17">OR(NOT(ISERROR(SEARCH($F$5,Q93))),Q93=0)*OR(NOT(ISERROR(SEARCH($F$6,R93))),R93=0)</f>
         <v>0</v>
       </c>
       <c r="P93" s="106"/>
@@ -45443,14 +45490,14 @@
         <v>0</v>
       </c>
       <c r="K94" s="150">
-        <f t="shared" ref="K94" si="19">SUM(H94*J94)</f>
+        <f t="shared" ref="K94" si="18">SUM(H94*J94)</f>
         <v>0</v>
       </c>
       <c r="L94" s="38"/>
       <c r="M94" s="104"/>
       <c r="N94" s="105"/>
       <c r="O94" s="106">
-        <f t="shared" ref="O94" si="20">OR(NOT(ISERROR(SEARCH($F$5,Q94))),Q94=0)*OR(NOT(ISERROR(SEARCH($F$6,R94))),R94=0)</f>
+        <f t="shared" ref="O94" si="19">OR(NOT(ISERROR(SEARCH($F$5,Q94))),Q94=0)*OR(NOT(ISERROR(SEARCH($F$6,R94))),R94=0)</f>
         <v>0</v>
       </c>
       <c r="P94" s="106"/>
@@ -45482,14 +45529,14 @@
         <v>0</v>
       </c>
       <c r="K95" s="150">
-        <f t="shared" ref="K95" si="21">SUM(H95*J95)</f>
+        <f t="shared" ref="K95" si="20">SUM(H95*J95)</f>
         <v>0</v>
       </c>
       <c r="L95" s="38"/>
       <c r="M95" s="104"/>
       <c r="N95" s="105"/>
       <c r="O95" s="106">
-        <f t="shared" ref="O95" si="22">OR(NOT(ISERROR(SEARCH($F$5,Q95))),Q95=0)*OR(NOT(ISERROR(SEARCH($F$6,R95))),R95=0)</f>
+        <f t="shared" ref="O95" si="21">OR(NOT(ISERROR(SEARCH($F$5,Q95))),Q95=0)*OR(NOT(ISERROR(SEARCH($F$6,R95))),R95=0)</f>
         <v>0</v>
       </c>
       <c r="P95" s="106"/>
@@ -45778,14 +45825,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K123" s="191" t="e">
-        <f t="shared" ref="K123:K129" ca="1" si="23">SUM(J123*H123)</f>
+        <f t="shared" ref="K123:K129" ca="1" si="22">SUM(J123*H123)</f>
         <v>#NAME?</v>
       </c>
       <c r="L123" s="38"/>
       <c r="M123" s="104"/>
       <c r="N123" s="40"/>
       <c r="O123" s="242">
-        <f t="shared" ref="O123:O129" si="24">OR(NOT(ISERROR(SEARCH($F$5,Q123))),Q123=0)*OR(NOT(ISERROR(SEARCH($F$6,R123))),R123=0)</f>
+        <f t="shared" ref="O123:O129" si="23">OR(NOT(ISERROR(SEARCH($F$5,Q123))),Q123=0)*OR(NOT(ISERROR(SEARCH($F$6,R123))),R123=0)</f>
         <v>1</v>
       </c>
       <c r="S123" s="108">
@@ -45813,14 +45860,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K124" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L124" s="38"/>
       <c r="M124" s="104"/>
       <c r="N124" s="40"/>
       <c r="O124" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S124" s="108">
@@ -45849,14 +45896,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K125" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L125" s="38"/>
       <c r="M125" s="104"/>
       <c r="N125" s="40"/>
       <c r="O125" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S125" s="108">
@@ -45885,14 +45932,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K126" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L126" s="38"/>
       <c r="M126" s="104"/>
       <c r="N126" s="40"/>
       <c r="O126" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S126" s="108">
@@ -45920,14 +45967,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K127" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L127" s="38"/>
       <c r="M127" s="104"/>
       <c r="N127" s="40"/>
       <c r="O127" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S127" s="108">
@@ -45956,14 +46003,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K128" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L128" s="38"/>
       <c r="M128" s="104"/>
       <c r="N128" s="40"/>
       <c r="O128" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="S128" s="108">
@@ -45991,14 +46038,14 @@
         <v>#NAME?</v>
       </c>
       <c r="K129" s="191" t="e">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#NAME?</v>
       </c>
       <c r="L129" s="38"/>
       <c r="M129" s="104"/>
       <c r="N129" s="40"/>
       <c r="O129" s="242">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="Q129" s="43" t="s">
@@ -46038,7 +46085,7 @@
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4:E4"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.9" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -46095,18 +46142,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="705" t="s">
+      <c r="E2" s="706" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="705"/>
+      <c r="F2" s="706"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="706" t="e">
+      <c r="J2" s="707" t="e">
         <f ca="1">SUMIF(O9:O235,"[",K9:K235)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="706"/>
+      <c r="K2" s="707"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -46116,10 +46163,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="707" t="s">
+      <c r="E3" s="708" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="707"/>
+      <c r="F3" s="708"/>
       <c r="G3" s="201"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -46379,7 +46426,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="708"/>
+      <c r="A14" s="709"/>
       <c r="B14" s="51"/>
       <c r="C14" s="7"/>
       <c r="D14" s="101"/>
@@ -46413,7 +46460,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="708"/>
+      <c r="A15" s="709"/>
       <c r="B15" s="51"/>
       <c r="C15" s="7"/>
       <c r="D15" s="101"/>
@@ -54319,7 +54366,7 @@
   <dimension ref="A1:N556"/>
   <sheetViews>
     <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -54439,7 +54486,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43327.35778726852</v>
+        <v>43333.416436111111</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>

</xml_diff>

<commit_message>
updates to template & code
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAjoku\Documents\GitHub\GCGRrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A141D-7B31-4F2B-A08D-9E00303D47B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F89745-1A36-451B-BA3D-94DD4B970E3C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="7020" xr2:uid="{2E80CA58-8610-40E9-A54D-09997D7EA2F4}"/>
   </bookViews>
@@ -82,6 +82,7 @@
     <definedName name="\c_negStart" localSheetId="2">'Staff Detail'!$M$1</definedName>
     <definedName name="\c_negTemp" localSheetId="2">'Staff Detail'!$AL$1</definedName>
     <definedName name="\c_order" localSheetId="2">'Staff Detail'!$S$1</definedName>
+    <definedName name="\c_OT" localSheetId="5">'Rate Tables'!$D$1</definedName>
     <definedName name="\c_perTIME" localSheetId="2">'Staff Detail'!$K$1</definedName>
     <definedName name="\c_posEnd" localSheetId="2">'Staff Detail'!$J$1</definedName>
     <definedName name="\c_Position" localSheetId="2">'Staff Detail'!$B$1</definedName>
@@ -97,6 +98,7 @@
     <definedName name="\c_region" localSheetId="7">'GRs Detail'!$Q$1</definedName>
     <definedName name="\c_report" localSheetId="6">'GCs Detail'!$B$1:$B$1</definedName>
     <definedName name="\c_report" localSheetId="7">'GRs Detail'!$B$1:$B$1</definedName>
+    <definedName name="\c_RT" localSheetId="5">'Rate Tables'!$C$1</definedName>
     <definedName name="\c_schedEnd" localSheetId="4">'Non-Staff Labor'!$X$1</definedName>
     <definedName name="\c_schedStart" localSheetId="4">'Non-Staff Labor'!$D$1</definedName>
     <definedName name="\c_SchedTemp" localSheetId="4">'Non-Staff Labor'!$AJ$1</definedName>
@@ -390,7 +392,7 @@
     <definedName name="staffcounter">Settings!$H$22</definedName>
     <definedName name="testg">Code!$J$8</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -505,7 +507,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="1015">
   <si>
     <t>Salary</t>
   </si>
@@ -3870,12 +3872,15 @@
   <si>
     <t>Carpenter Foreman</t>
   </si>
+  <si>
+    <t>Starting Rate:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="24">
+  <numFmts count="25">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -3900,8 +3905,9 @@
     <numFmt numFmtId="181" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="182" formatCode="###,###,###"/>
     <numFmt numFmtId="183" formatCode="0#####"/>
+    <numFmt numFmtId="184" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* &quot;-&quot;_);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="87" x14ac:knownFonts="1">
+  <fonts count="88" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4488,6 +4494,13 @@
     <font>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -6090,7 +6103,7 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="710">
+  <cellXfs count="712">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -8121,20 +8134,23 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="44" fontId="65" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="77" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="87" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -8158,6 +8174,22 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="2"/>
       <protection locked="0"/>
@@ -8166,14 +8198,6 @@
       <alignment horizontal="left" vertical="top" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -8195,14 +8219,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -19825,22 +19841,22 @@
       <definedName name="dummy"/>
     </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -20409,8 +20425,8 @@
       <c r="C4" s="314" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="687"/>
-      <c r="E4" s="688"/>
+      <c r="D4" s="689"/>
+      <c r="E4" s="690"/>
       <c r="F4" s="315"/>
       <c r="G4" s="314" t="s">
         <v>207</v>
@@ -20437,8 +20453,8 @@
       <c r="C5" s="314" t="s">
         <v>215</v>
       </c>
-      <c r="D5" s="687"/>
-      <c r="E5" s="688"/>
+      <c r="D5" s="689"/>
+      <c r="E5" s="690"/>
       <c r="F5" s="315"/>
       <c r="G5" s="314" t="s">
         <v>208</v>
@@ -20465,10 +20481,10 @@
       <c r="C6" s="314" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="687" t="s">
+      <c r="D6" s="689" t="s">
         <v>274</v>
       </c>
-      <c r="E6" s="688"/>
+      <c r="E6" s="690"/>
       <c r="F6" s="315"/>
       <c r="G6" s="314" t="s">
         <v>9</v>
@@ -20478,7 +20494,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I6" s="315"/>
-      <c r="J6" s="689" t="s">
+      <c r="J6" s="691" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="514" t="e">
@@ -20501,10 +20517,10 @@
       <c r="C7" s="314" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="685" t="s">
+      <c r="D7" s="687" t="s">
         <v>282</v>
       </c>
-      <c r="E7" s="686"/>
+      <c r="E7" s="688"/>
       <c r="F7" s="315"/>
       <c r="G7" s="315"/>
       <c r="H7" s="515" t="e">
@@ -20512,7 +20528,7 @@
         <v>#NAME?</v>
       </c>
       <c r="I7" s="318"/>
-      <c r="J7" s="689"/>
+      <c r="J7" s="691"/>
       <c r="K7" s="515" t="e">
         <f ca="1">IF(cDateDiff("WW",\cstart,\cend)&gt;0,cDateDiff("WW",\cstart,\cend),0)</f>
         <v>#NAME?</v>
@@ -20604,7 +20620,7 @@
       </c>
       <c r="D11" s="12">
         <f ca="1">NOW()</f>
-        <v>43333.416436111111</v>
+        <v>43334.447860995373</v>
       </c>
       <c r="E11" s="315"/>
       <c r="F11" s="313"/>
@@ -20722,10 +20738,10 @@
       <c r="C16" s="314" t="s">
         <v>227</v>
       </c>
-      <c r="D16" s="687" t="s">
+      <c r="D16" s="689" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="688"/>
+      <c r="E16" s="690"/>
       <c r="F16" s="315"/>
       <c r="G16" s="314" t="s">
         <v>226</v>
@@ -21100,7 +21116,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43333.416436111111</v>
+        <v>43334.447860995373</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>
@@ -34544,10 +34560,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -34628,11 +34644,11 @@
       <c r="AM1" s="321"/>
     </row>
     <row r="2" spans="1:43" s="311" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="690" t="str">
+      <c r="B2" s="696" t="str">
         <f>IF(Settings!D4&lt;&gt;0,Settings!D4,"")</f>
         <v/>
       </c>
-      <c r="C2" s="690"/>
+      <c r="C2" s="696"/>
       <c r="D2" s="324"/>
       <c r="G2" s="325"/>
       <c r="AB2" s="326"/>
@@ -34644,15 +34660,15 @@
       <c r="AQ2" s="321"/>
     </row>
     <row r="3" spans="1:43" s="311" customFormat="1" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="691" t="str">
+      <c r="B3" s="697" t="str">
         <f>IF(Settings!D5&lt;&gt;0,Settings!D5,"")</f>
         <v/>
       </c>
-      <c r="C3" s="691"/>
+      <c r="C3" s="697"/>
       <c r="D3" s="327"/>
       <c r="E3" s="328">
         <f ca="1">Settings!\date</f>
-        <v>43333.416436111111</v>
+        <v>43334.447860995373</v>
       </c>
       <c r="Q3" s="326"/>
       <c r="AD3" s="326"/>
@@ -34879,18 +34895,18 @@
       <c r="B11" s="351"/>
       <c r="C11" s="352"/>
       <c r="D11" s="352"/>
-      <c r="E11" s="694" t="s">
+      <c r="E11" s="698" t="s">
         <v>245</v>
       </c>
       <c r="F11" s="352"/>
-      <c r="G11" s="694" t="s">
+      <c r="G11" s="698" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="352"/>
-      <c r="I11" s="694" t="s">
+      <c r="I11" s="698" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="694" t="s">
+      <c r="J11" s="698" t="s">
         <v>246</v>
       </c>
       <c r="K11" s="353"/>
@@ -34902,13 +34918,13 @@
       </c>
       <c r="O11" s="359"/>
       <c r="P11" s="360"/>
-      <c r="Q11" s="696" t="s">
+      <c r="Q11" s="700" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="700" t="s">
+      <c r="R11" s="694" t="s">
         <v>368</v>
       </c>
-      <c r="S11" s="698" t="s">
+      <c r="S11" s="702" t="s">
         <v>369</v>
       </c>
       <c r="T11" s="692" t="s">
@@ -34959,14 +34975,14 @@
       <c r="D12" s="365" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="695"/>
+      <c r="E12" s="699"/>
       <c r="F12" s="365"/>
-      <c r="G12" s="695"/>
+      <c r="G12" s="699"/>
       <c r="H12" s="365" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="695"/>
-      <c r="J12" s="695"/>
+      <c r="I12" s="699"/>
+      <c r="J12" s="699"/>
       <c r="K12" s="366" t="s">
         <v>232</v>
       </c>
@@ -34981,9 +34997,9 @@
       <c r="P12" s="373" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="697"/>
-      <c r="R12" s="701"/>
-      <c r="S12" s="699"/>
+      <c r="Q12" s="701"/>
+      <c r="R12" s="695"/>
+      <c r="S12" s="703"/>
       <c r="T12" s="693"/>
       <c r="U12" s="693"/>
       <c r="V12" s="693"/>
@@ -37514,13 +37530,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
   <mergeCells count="18">
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="W11:W12"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="U11:U12"/>
@@ -37532,6 +37541,13 @@
     <mergeCell ref="Q11:Q12"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="S11:S12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="W11:W12"/>
   </mergeCells>
   <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="11" priority="4">
@@ -37565,7 +37581,7 @@
   <dimension ref="A1:CR193"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -37585,22 +37601,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="I1" s="702"/>
-      <c r="J1" s="702"/>
-      <c r="K1" s="702"/>
-      <c r="L1" s="702"/>
-      <c r="M1" s="702"/>
-      <c r="N1" s="702"/>
-      <c r="O1" s="702"/>
-      <c r="P1" s="702"/>
-      <c r="Q1" s="702"/>
-      <c r="R1" s="702"/>
-      <c r="S1" s="702"/>
-      <c r="T1" s="702"/>
-      <c r="U1" s="702"/>
-      <c r="V1" s="702"/>
-      <c r="W1" s="702"/>
-      <c r="X1" s="702"/>
+      <c r="I1" s="704"/>
+      <c r="J1" s="704"/>
+      <c r="K1" s="704"/>
+      <c r="L1" s="704"/>
+      <c r="M1" s="704"/>
+      <c r="N1" s="704"/>
+      <c r="O1" s="704"/>
+      <c r="P1" s="704"/>
+      <c r="Q1" s="704"/>
+      <c r="R1" s="704"/>
+      <c r="S1" s="704"/>
+      <c r="T1" s="704"/>
+      <c r="U1" s="704"/>
+      <c r="V1" s="704"/>
+      <c r="W1" s="704"/>
+      <c r="X1" s="704"/>
       <c r="Y1" s="608"/>
       <c r="Z1" s="608"/>
       <c r="AA1" s="608"/>
@@ -37644,6 +37660,7 @@
     <row r="6" spans="1:96" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I6" s="610"/>
       <c r="AE6" s="611"/>
+      <c r="CR6" s="612"/>
     </row>
     <row r="7" spans="1:96" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="612"/>
@@ -38002,7 +38019,7 @@
         <v>85</v>
       </c>
       <c r="CP7" s="623"/>
-      <c r="CR7" s="615">
+      <c r="CR7" s="682">
         <f>CQ7+1</f>
         <v>1</v>
       </c>
@@ -38101,7 +38118,7 @@
       <c r="CL8" s="634"/>
       <c r="CM8" s="634"/>
       <c r="CN8" s="634"/>
-      <c r="CO8" s="634"/>
+      <c r="CO8" s="639"/>
       <c r="CP8" s="623"/>
       <c r="CR8" s="634"/>
     </row>
@@ -38324,7 +38341,7 @@
       </c>
       <c r="G11" s="651"/>
       <c r="H11" s="652"/>
-      <c r="I11" s="683"/>
+      <c r="I11" s="681"/>
       <c r="J11" s="607"/>
       <c r="K11" s="607"/>
       <c r="L11" s="607"/>
@@ -38408,9 +38425,9 @@
       <c r="CL11" s="607"/>
       <c r="CM11" s="607"/>
       <c r="CN11" s="607"/>
-      <c r="CO11" s="684"/>
+      <c r="CO11" s="686"/>
       <c r="CP11" s="623"/>
-      <c r="CR11" s="681"/>
+      <c r="CR11" s="607"/>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.25">
       <c r="B12" s="606"/>
@@ -39394,7 +39411,7 @@
   <dimension ref="A1:AM19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39424,27 +39441,72 @@
     <col min="23" max="23" width="12.7109375" style="9" customWidth="1"/>
     <col min="24" max="34" width="9.140625" style="9"/>
     <col min="35" max="35" width="9" style="9" customWidth="1"/>
-    <col min="36" max="36" width="11.42578125" style="9" customWidth="1"/>
-    <col min="37" max="37" width="7.85546875" style="9" customWidth="1"/>
-    <col min="38" max="38" width="7.28515625" style="9" customWidth="1"/>
-    <col min="39" max="40" width="9.140625" style="9" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" style="9" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="7.85546875" style="9" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="7.28515625" style="9" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" style="9" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="9" customWidth="1"/>
     <col min="41" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="U1" s="703"/>
-      <c r="V1" s="703"/>
-      <c r="W1" s="703"/>
-      <c r="AJ1" s="703"/>
-      <c r="AK1" s="703"/>
-      <c r="AL1" s="703"/>
-      <c r="AM1" s="703"/>
+      <c r="U1" s="705"/>
+      <c r="V1" s="705"/>
+      <c r="W1" s="705"/>
+      <c r="AJ1" s="705"/>
+      <c r="AK1" s="705"/>
+      <c r="AL1" s="705"/>
+      <c r="AM1" s="705"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="H6" s="672"/>
       <c r="I6" s="57"/>
       <c r="J6" s="57"/>
     </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G9" s="685">
+        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$5:$D$8,MATCH(OFFSET($E12,1,0),'Rate Tables'!$B$5:$B$8,-1),2),INDEX('Rate Tables'!$B$5:$D$8,1,2))</f>
+        <v>97.75</v>
+      </c>
+      <c r="I9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J9" s="685">
+        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$19:$D$22,MATCH(OFFSET($E12,1,0),'Rate Tables'!$B$19:$B$22,-1),2),INDEX('Rate Tables'!$B$19:$D$22,1,2))</f>
+        <v>118</v>
+      </c>
+      <c r="L9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="M9" s="685">
+        <f>INDEX('Rate Tables'!$B$33:$D$33,1,2)</f>
+        <v>45</v>
+      </c>
+      <c r="O9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="P9" s="685">
+        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$37:$D$40,MATCH(OFFSET($E12,1,0),'Rate Tables'!$B$37:$B$40,-1),2),INDEX('Rate Tables'!$B$37:$D$40,1,2))</f>
+        <v>1</v>
+      </c>
+      <c r="R9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="S9" s="685">
+        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$44:$D$47,MATCH(OFFSET($E12,1,0),'Rate Tables'!$B$44:$B$47,-1),2),INDEX('Rate Tables'!$B$44:$D$47,1,2))</f>
+        <v>1</v>
+      </c>
+      <c r="U9" s="684" t="s">
+        <v>1014</v>
+      </c>
+      <c r="V9" s="685">
+        <f>INDEX('Rate Tables'!$B$51:$D$51,1,2)</f>
+        <v>45</v>
+      </c>
+    </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L10" s="185"/>
     </row>
@@ -39452,43 +39514,43 @@
       <c r="C11" s="57"/>
       <c r="D11" s="264"/>
       <c r="E11" s="265"/>
-      <c r="F11" s="704" t="s">
+      <c r="F11" s="706" t="s">
         <v>1009</v>
       </c>
-      <c r="G11" s="704"/>
-      <c r="H11" s="704"/>
-      <c r="I11" s="705" t="s">
+      <c r="G11" s="706"/>
+      <c r="H11" s="706"/>
+      <c r="I11" s="707" t="s">
         <v>470</v>
       </c>
-      <c r="J11" s="705"/>
-      <c r="K11" s="705"/>
-      <c r="L11" s="705" t="s">
+      <c r="J11" s="707"/>
+      <c r="K11" s="707"/>
+      <c r="L11" s="707" t="s">
         <v>364</v>
       </c>
-      <c r="M11" s="705"/>
-      <c r="N11" s="705"/>
-      <c r="O11" s="705" t="s">
+      <c r="M11" s="707"/>
+      <c r="N11" s="707"/>
+      <c r="O11" s="707" t="s">
         <v>1010</v>
       </c>
-      <c r="P11" s="705"/>
-      <c r="Q11" s="705"/>
-      <c r="R11" s="705" t="s">
+      <c r="P11" s="707"/>
+      <c r="Q11" s="707"/>
+      <c r="R11" s="707" t="s">
         <v>1011</v>
       </c>
-      <c r="S11" s="705"/>
-      <c r="T11" s="705"/>
-      <c r="U11" s="705" t="s">
+      <c r="S11" s="707"/>
+      <c r="T11" s="707"/>
+      <c r="U11" s="707" t="s">
         <v>79</v>
       </c>
-      <c r="V11" s="705"/>
-      <c r="W11" s="705"/>
+      <c r="V11" s="707"/>
+      <c r="W11" s="707"/>
       <c r="X11" s="56"/>
-      <c r="AJ11" s="705" t="s">
+      <c r="AJ11" s="707" t="s">
         <v>373</v>
       </c>
-      <c r="AK11" s="705"/>
-      <c r="AL11" s="705"/>
-      <c r="AM11" s="705"/>
+      <c r="AK11" s="707"/>
+      <c r="AL11" s="707"/>
+      <c r="AM11" s="707"/>
     </row>
     <row r="12" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="57"/>
@@ -39567,7 +39629,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C13" s="682"/>
+      <c r="C13" s="680"/>
       <c r="D13" s="262" t="s">
         <v>407</v>
       </c>
@@ -39626,13 +39688,13 @@
       <c r="E14" s="175"/>
       <c r="F14" s="175"/>
       <c r="G14" s="533"/>
-      <c r="H14" s="679">
+      <c r="H14" s="678">
         <f t="array" aca="1" ref="H14" ca="1">IFERROR(SUM((IF((OFFSET(F12,1,0):OFFSET(F13,-1,0)&lt;=1)*(OFFSET(F12,1,0):OFFSET(F13,-1,0)&gt;0),OFFSET(F12,1,0):OFFSET(F13,-1,0),IF(OFFSET(F12,1,0):OFFSET(F13,-1,0)&gt;1,1,0)))*40*IFERROR(INDEX('Rate Tables'!$B$12:$D$15,MATCH(OFFSET($E12,1,0):OFFSET($E13,-1,0),'Rate Tables'!$B$12:$B$15,-1),2),INDEX('Rate Tables'!$B$12:$D$15,1,2)) +(OFFSET(G12,1,0):OFFSET(G13,-1,0))*40*IFERROR(INDEX('Rate Tables'!$B$12:$D$15,MATCH(OFFSET($E12,1,0):OFFSET($E13,-1,0),'Rate Tables'!$B$12:$B$15,-1),3),INDEX('Rate Tables'!$B$12:$D$15,1,3)) ),0)</f>
         <v>0</v>
       </c>
       <c r="I14" s="534"/>
       <c r="J14" s="668"/>
-      <c r="K14" s="679">
+      <c r="K14" s="678">
         <f t="array" aca="1" ref="K14" ca="1">IFERROR(SUM((IF((OFFSET(I12,1,0):OFFSET(I13,-1,0)&lt;=1)*(OFFSET(I12,1,0):OFFSET(I13,-1,0)&gt;0),OFFSET(I12,1,0):OFFSET(I13,-1,0),IF(OFFSET(I12,1,0):OFFSET(I13,-1,0)&gt;1,1,0)))*40*IFERROR(INDEX('Rate Tables'!$B$26:$D$29,MATCH(OFFSET($E12,1,0):OFFSET($E13,-1,0),'Rate Tables'!$B$26:$B$29,-1),2),INDEX('Rate Tables'!$B$26:$D$29,1,2)) +(OFFSET(J12,1,0):OFFSET(J13,-1,0))*40*IFERROR(INDEX('Rate Tables'!$B$26:$D$29,MATCH(OFFSET($E12,1,0):OFFSET($E13,-1,0),'Rate Tables'!$B$26:$B$29,-1),3),INDEX('Rate Tables'!$B$26:$D$29,1,3)) ),0)</f>
         <v>0</v>
       </c>
@@ -39663,13 +39725,13 @@
       <c r="F15" s="60"/>
       <c r="G15" s="537"/>
       <c r="H15" s="133">
-        <f ca="1">SUM(H13:H14)</f>
+        <f ca="1">SUM(H13)</f>
         <v>0</v>
       </c>
       <c r="I15" s="60"/>
       <c r="J15" s="537"/>
       <c r="K15" s="133">
-        <f ca="1">SUM(K13:K14)</f>
+        <f ca="1">SUM(K13)</f>
         <v>0</v>
       </c>
       <c r="L15" s="60"/>
@@ -39751,7 +39813,7 @@
       <c r="T17" s="57"/>
     </row>
     <row r="19" spans="1:39" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="680"/>
+      <c r="A19" s="679"/>
       <c r="C19" s="669"/>
       <c r="D19" s="180">
         <f ca="1">IFERROR(OFFSET(D19,-1,0)+1,1)</f>
@@ -39763,38 +39825,38 @@
       </c>
       <c r="F19" s="182"/>
       <c r="G19" s="673"/>
-      <c r="H19" s="678">
-        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$5:$D$8,MATCH($E19,'Rate Tables'!$B$5:$B$8,-1),2),INDEX('Rate Tables'!$B$5:$D$8,1,2))*40*F19+((40*G19)*IFERROR(INDEX('Rate Tables'!$B$5:$D$8,MATCH($E19,'Rate Tables'!$B$5:$B$8,-1),3),INDEX('Rate Tables'!$B$5:$D$8,1,3)))</f>
-        <v>0</v>
+      <c r="H19" s="683">
+        <f ca="1">(IF(AND(F19&gt;0,F19&lt;=1),F19,IF(F19&gt;1,1,0))*(40*IFERROR(INDEX('Rate Tables'!$B$12:$D$15,MATCH($E19,'Rate Tables'!$B$12:$B$15,-1),2),INDEX('Rate Tables'!$B$12:$D$15,1,2))+(G19*40*IFERROR(INDEX('Rate Tables'!$B$12:$D$15,MATCH($E19,'Rate Tables'!$B$12:$B$15,-1),3),INDEX('Rate Tables'!$B$12:$D$15,1,3))))+((F19-1)*((IFERROR(INDEX('Rate Tables'!$B$5:$D$8,MATCH($E19,'Rate Tables'!$B$5:$B$8,-1),2),INDEX('Rate Tables'!$B$5:$D$8,1,2))*40)+(40*G19*IFERROR(INDEX('Rate Tables'!$B$5:$D$8,MATCH($E19,'Rate Tables'!$B$5:$B$8,-1),3),INDEX('Rate Tables'!$B$5:$D$8,1,3))))))</f>
+        <v>-3910</v>
       </c>
       <c r="I19" s="183"/>
       <c r="J19" s="673"/>
-      <c r="K19" s="678">
-        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$19:$D$22,MATCH($E19,'Rate Tables'!$B$19:$B$22,-1),2),INDEX('Rate Tables'!$B$19:$D$22,1,2))*40*I19+((40*J19)*IFERROR(INDEX('Rate Tables'!$B$19:$D$22,MATCH($E19,'Rate Tables'!$B$19:$B$22,-1),3),INDEX('Rate Tables'!$B$19:$D$22,1,3)))</f>
-        <v>0</v>
+      <c r="K19" s="683">
+        <f ca="1">(IF(AND(I19&gt;0,I19&lt;=1),I19,IF(I19&gt;1,1,0))*(40*IFERROR(INDEX('Rate Tables'!$B$26:$D$29,MATCH($E19,'Rate Tables'!$B$26:$B$29,-1),2),INDEX('Rate Tables'!$B$26:$D$29,1,2)) +(J19*40*IFERROR(INDEX('Rate Tables'!$B$26:$D$29,MATCH($E19,'Rate Tables'!$B$26:$B$29,-1),3),INDEX('Rate Tables'!$B$26:$D$29,1,3)))) + ((I19-1)*((IFERROR(INDEX('Rate Tables'!$B$19:$D$22,MATCH($E19,'Rate Tables'!$B$19:$B$22,-1),2),INDEX('Rate Tables'!$B$19:$D$22,1,2))*40)+(40*J19*IFERROR(INDEX('Rate Tables'!$B$19:$D$22,MATCH($E19,'Rate Tables'!$B$19:$B$22,-1),3),INDEX('Rate Tables'!$B$19:$D$22,1,3))))))</f>
+        <v>-4720</v>
       </c>
       <c r="L19" s="183"/>
       <c r="M19" s="673"/>
-      <c r="N19" s="678">
-        <f>INDEX('Rate Tables'!$B$33:$D$33,1,2)*40*L19+((40*M19)*INDEX('Rate Tables'!$B$33:$D$33,1,3))</f>
+      <c r="N19" s="184">
+        <f>L19*(INDEX('Rate Tables'!$B$33:$D$33,1,2)*40+((40*M19)*INDEX('Rate Tables'!$B$33:$D$33,1,3)))</f>
         <v>0</v>
       </c>
       <c r="O19" s="183"/>
       <c r="P19" s="673"/>
-      <c r="Q19" s="678">
-        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$37:$D$40,MATCH($E19,'Rate Tables'!$B$37:$B$40,-1),2),INDEX('Rate Tables'!$B$37:$D$40,1,2))*40*O19+((40*P19)*IFERROR(INDEX('Rate Tables'!$B$37:$D$40,MATCH($E19,'Rate Tables'!$B$37:$B$40,-1),3),INDEX('Rate Tables'!$B$37:$D$40,1,3)))</f>
+      <c r="Q19" s="184">
+        <f ca="1">O19*(IFERROR(INDEX('Rate Tables'!$B$37:$D$40,MATCH($E19,'Rate Tables'!$B$37:$B$40,-1),2),INDEX('Rate Tables'!$B$37:$D$40,1,2))*40+((40*P19)*IFERROR(INDEX('Rate Tables'!$B$37:$D$40,MATCH($E19,'Rate Tables'!$B$37:$B$40,-1),3),INDEX('Rate Tables'!$B$37:$D$40,1,3))))</f>
         <v>0</v>
       </c>
       <c r="R19" s="183"/>
       <c r="S19" s="673"/>
-      <c r="T19" s="678">
-        <f ca="1">IFERROR(INDEX('Rate Tables'!$B$44:$D$47,MATCH($E19,'Rate Tables'!$B$44:$B$47,-1),2),INDEX('Rate Tables'!$B$44:$D$47,1,2))*40*R19+((40*S19)*IFERROR(INDEX('Rate Tables'!$B$44:$D$47,MATCH($E19,'Rate Tables'!$B$44:$B$47,-1),3),INDEX('Rate Tables'!$B$44:$D$47,1,3)))</f>
+      <c r="T19" s="184">
+        <f ca="1">R19*(IFERROR(INDEX('Rate Tables'!$B$44:$D$47,MATCH($E19,'Rate Tables'!$B$44:$B$47,-1),2),INDEX('Rate Tables'!$B$44:$D$47,1,2))*40+((40*S19)*IFERROR(INDEX('Rate Tables'!$B$44:$D$47,MATCH($E19,'Rate Tables'!$B$44:$B$47,-1),3),INDEX('Rate Tables'!$B$44:$D$47,1,3))))</f>
         <v>0</v>
       </c>
       <c r="U19" s="183"/>
       <c r="V19" s="673"/>
-      <c r="W19" s="678">
-        <f>INDEX('Rate Tables'!$B$51:$D$51,1,2)*40*U19+((40*V19)*INDEX('Rate Tables'!$B$51:$D$51,1,3))</f>
+      <c r="W19" s="184">
+        <f>U19*(INDEX('Rate Tables'!$B$51:$D$51,1,2)*40+((40*V19)*INDEX('Rate Tables'!$B$51:$D$51,1,3)))</f>
         <v>0</v>
       </c>
       <c r="X19" s="56"/>
@@ -39833,10 +39895,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A12B0C-DA54-4CAA-B658-BD043332B91F}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A2:Y51"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39851,6 +39913,10 @@
     <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C1" s="413"/>
+      <c r="D1" s="413"/>
+    </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B2" s="671"/>
     </row>
@@ -42539,18 +42605,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="706" t="s">
+      <c r="E2" s="708" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="706"/>
+      <c r="F2" s="708"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="707" t="e">
+      <c r="J2" s="709" t="e">
         <f ca="1">SUMIF(O9:O100,"[",K9:K100)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="707"/>
+      <c r="K2" s="709"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -42560,10 +42626,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="708" t="s">
+      <c r="E3" s="710" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="708"/>
+      <c r="F3" s="710"/>
       <c r="G3" s="135"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -46142,18 +46208,18 @@
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="706" t="s">
+      <c r="E2" s="708" t="s">
         <v>384</v>
       </c>
-      <c r="F2" s="706"/>
+      <c r="F2" s="708"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="131"/>
-      <c r="J2" s="707" t="e">
+      <c r="J2" s="709" t="e">
         <f ca="1">SUMIF(O9:O235,"[",K9:K235)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K2" s="707"/>
+      <c r="K2" s="709"/>
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
       <c r="N2" s="19"/>
@@ -46163,10 +46229,10 @@
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="57"/>
-      <c r="E3" s="708" t="s">
+      <c r="E3" s="710" t="s">
         <v>384</v>
       </c>
-      <c r="F3" s="708"/>
+      <c r="F3" s="710"/>
       <c r="G3" s="201"/>
       <c r="H3" s="57"/>
       <c r="I3" s="57"/>
@@ -46426,7 +46492,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="709"/>
+      <c r="A14" s="711"/>
       <c r="B14" s="51"/>
       <c r="C14" s="7"/>
       <c r="D14" s="101"/>
@@ -46460,7 +46526,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="709"/>
+      <c r="A15" s="711"/>
       <c r="B15" s="51"/>
       <c r="C15" s="7"/>
       <c r="D15" s="101"/>
@@ -54486,7 +54552,7 @@
       <c r="K7" s="562"/>
       <c r="L7" s="563">
         <f ca="1">Settings!\date</f>
-        <v>43333.416436111111</v>
+        <v>43334.447860995373</v>
       </c>
       <c r="M7" s="564"/>
       <c r="N7" s="498"/>

</xml_diff>